<commit_message>
Contains Duplicate 1 & 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D240A7-B9F6-43C6-8A05-036ECD671BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D97776F-8E96-46C2-8F9A-451B8D707206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Id</t>
   </si>
@@ -103,6 +103,33 @@
   </si>
   <si>
     <t>have 2 hashmaps, loop check each key in each string, add them in the corresponding maps, check for values.</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Walk and push to a stack, pop the stack</t>
+  </si>
+  <si>
+    <t>move 3 ptrs switch direction or recursive (prev,current)</t>
+  </si>
+  <si>
+    <t>Stack/3 Ptrs/Recursive</t>
+  </si>
+  <si>
+    <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>HashSet/Array.Sort/Old school O(n^2)</t>
+  </si>
+  <si>
+    <t>Contains Duplicate 2</t>
+  </si>
+  <si>
+    <t>HashMap/Dictionary/unordered_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have a map, loop add key, if key exists check abs value with n, return true, else assign new index to current map value. </t>
   </si>
 </sst>
 </file>
@@ -420,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +582,48 @@
         <v>25</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>206</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>217</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>219</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find The Original Typed String 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A92EAB-F1A6-4CD4-8540-6EF9151D9D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2F4B1D-3BB3-4001-A17A-7499413C58F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="4365" windowWidth="15270" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Id</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>Find mid, reverse, compare</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t>Contain char c and Remove char c</t>
+  </si>
+  <si>
+    <t>Frequency Table/List/LinQ/HashMap</t>
+  </si>
+  <si>
+    <t>Frequency table ++ --, 2 HashMap ++  and compare them</t>
+  </si>
+  <si>
+    <t>Find the original typed string</t>
+  </si>
+  <si>
+    <t>Frequency Table/Skip/Compare prev</t>
   </si>
 </sst>
 </file>
@@ -507,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>232</v>
       </c>
@@ -768,7 +786,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>234</v>
       </c>
@@ -780,6 +798,34 @@
       </c>
       <c r="D18" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>242</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3330</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find The Original Typed String 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2F4B1D-3BB3-4001-A17A-7499413C58F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E55525A-5A99-4508-9D6F-A5E7E7C38CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7035" yWindow="2010" windowWidth="15270" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Id</t>
   </si>
@@ -204,10 +204,22 @@
     <t>Frequency table ++ --, 2 HashMap ++  and compare them</t>
   </si>
   <si>
-    <t>Find the original typed string</t>
-  </si>
-  <si>
     <t>Frequency Table/Skip/Compare prev</t>
+  </si>
+  <si>
+    <t>Find the original typed string 1</t>
+  </si>
+  <si>
+    <t>Math/Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Find the original typed string 2</t>
+  </si>
+  <si>
+    <t>Have an array of letter_groups count(same letter possiblility), compute totalCombination from each group, find number of invalid value for each group in an array, return the result - invalid value with MOD guard.</t>
+  </si>
+  <si>
+    <t>Binary Tree Paths</t>
   </si>
 </sst>
 </file>
@@ -525,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +834,35 @@
         <v>3330</v>
       </c>
       <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
-        <v>60</v>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3333</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>257</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find The K-th Character in String Game 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCA0671-8147-415A-9C26-E673CDBD4C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AEAD61-F72E-4BAC-BF78-EEFD46F2D5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7035" yWindow="2010" windowWidth="15270" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Id</t>
   </si>
@@ -223,6 +223,27 @@
   </si>
   <si>
     <t>make a void util function(root,list,path), base case stop and add the string to the list, and traverse left and right.</t>
+  </si>
+  <si>
+    <t>Add Digits</t>
+  </si>
+  <si>
+    <t>Recursion/Loop/</t>
+  </si>
+  <si>
+    <t>while in while,</t>
+  </si>
+  <si>
+    <t>Find the K-th Character in String Game 1</t>
+  </si>
+  <si>
+    <t>Recursion/Loop/Math</t>
+  </si>
+  <si>
+    <t>1+((num-1) % 9)</t>
+  </si>
+  <si>
+    <t>Generate word with StringBuilder, return the result[k-1].</t>
   </si>
 </sst>
 </file>
@@ -540,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,6 +892,37 @@
         <v>65</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>258</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3304</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find the K-th Character in String Game 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD0C8CA-2C69-43F5-8A46-58022BDFC3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19D9A37-0CC9-4B31-83F6-FA7876DEA5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="2010" windowWidth="19695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>Loop in loop to search the unavailable number from the range of 0 -&gt; n</t>
+  </si>
+  <si>
+    <t>Find the K-th Character in String Game 2</t>
+  </si>
+  <si>
+    <t>Exponential growth/Math/Reverse</t>
+  </si>
+  <si>
+    <t>Find the smallest n length and number of operations to reach k | Reverse the operation because the string grows exponentially(double). K is unaffected if it's in the first half of the current string. | Zoom-in the first half aka search in first half reversly to locate k. Continue until k is in first half. | Trim the first half to find new k-th position in the second half.</t>
+  </si>
+  <si>
+    <t>Same logic, with if instead of switch case</t>
   </si>
 </sst>
 </file>
@@ -582,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,6 +987,23 @@
         <v>79</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3307</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find The Lucky Integer in an Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35A4422-B93F-4328-96AE-163B8F5BC2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A8E1C3-D01B-4C6E-8F32-C6F2E50B6BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="2010" windowWidth="19695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
     <t>Id</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>1 hash map, contains key and contains value comparision. CPP split words with iss &lt;sstream&gt;.</t>
+  </si>
+  <si>
+    <t>Find Lucky Integer in an Array</t>
+  </si>
+  <si>
+    <t>Frequency Table/Dictionary</t>
+  </si>
+  <si>
+    <t>make a freq table[arr.Length] because the lucky number must be equal to or less than the Length. Foreach to count freq, reverse loop to return the highest</t>
+  </si>
+  <si>
+    <t>have a hashmap, count the kvp, extract the highest key from the hashmap.</t>
   </si>
 </sst>
 </file>
@@ -624,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,6 +1094,23 @@
         <v>93</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1394</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nim Game & Range Sum Query - Immutable.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A8E1C3-D01B-4C6E-8F32-C6F2E50B6BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52306443-2E9E-41C2-ABF8-B3B6A3C247AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="2010" windowWidth="19695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
   <si>
     <t>Id</t>
   </si>
@@ -319,6 +319,27 @@
   </si>
   <si>
     <t>have a hashmap, count the kvp, extract the highest key from the hashmap.</t>
+  </si>
+  <si>
+    <t>Nim Game</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Multiples of 4.</t>
+  </si>
+  <si>
+    <t>Range Sum Query - Immutable</t>
+  </si>
+  <si>
+    <t>Math/Query</t>
+  </si>
+  <si>
+    <t>Culmulative sum for field initialization, because it's a query with multiple calls, we want optimal exec time for the method in O(1), not O(n).</t>
+  </si>
+  <si>
+    <t>in CPP we can use vector.back().</t>
   </si>
 </sst>
 </file>
@@ -636,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1132,37 @@
         <v>97</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>292</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>303</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finding Pairs with a certain Sum.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52306443-2E9E-41C2-ABF8-B3B6A3C247AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED55ADA-AD48-40CA-8F10-8B757CEBC399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="2010" windowWidth="19695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
   <si>
     <t>Id</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Find Lucky Integer in an Array</t>
   </si>
   <si>
-    <t>Frequency Table/Dictionary</t>
-  </si>
-  <si>
     <t>make a freq table[arr.Length] because the lucky number must be equal to or less than the Length. Foreach to count freq, reverse loop to return the highest</t>
   </si>
   <si>
@@ -340,6 +337,21 @@
   </si>
   <si>
     <t>in CPP we can use vector.back().</t>
+  </si>
+  <si>
+    <t>Finding Pairs with a Certain sum</t>
+  </si>
+  <si>
+    <t>Frequency Table/Dictionary/HashMap</t>
+  </si>
+  <si>
+    <t>HashMap/Dictionary/Frequency Table</t>
+  </si>
+  <si>
+    <t>2 int arrays and a Dictionary&lt;int,int&gt; frequency table, update the frequency table in Add(), search the complement key in Count</t>
+  </si>
+  <si>
+    <t>C# Remove() = CPP erase()</t>
   </si>
 </sst>
 </file>
@@ -657,15 +669,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="135.140625" customWidth="1"/>
     <col min="5" max="5" width="163.5703125" bestFit="1" customWidth="1"/>
@@ -1123,13 +1135,13 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
         <v>95</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>96</v>
-      </c>
-      <c r="E31" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,13 +1149,13 @@
         <v>292</v>
       </c>
       <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
         <v>98</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>99</v>
-      </c>
-      <c r="D32" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1151,16 +1163,33 @@
         <v>303</v>
       </c>
       <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
         <v>101</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>102</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>103</v>
       </c>
-      <c r="E33" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1865</v>
+      </c>
+      <c r="B34" t="s">
         <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maximum Number of Events That Can Be Attended.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF17066-53D0-45A2-9825-F66D9296C301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDFB305-C916-4FD2-9D74-6CD7E47BA734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="2010" windowWidth="19695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
   <si>
     <t>Id</t>
   </si>
@@ -358,6 +358,21 @@
   </si>
   <si>
     <t>MAX_POWER = 3^19 = 1162261467, the rest are factors.</t>
+  </si>
+  <si>
+    <t>Maximum Number of Events That Can Be Attended</t>
+  </si>
+  <si>
+    <t>Sort/Math/Greedy Strategy/Min-Heap/Priority Queue</t>
+  </si>
+  <si>
+    <t>Sort the events in chronological order, have a min-heap(PriorityQueue), while there is still an event left in events or the heap empty, iterate to add valid attendable events to the heap, remove the expired events, pop and count (attend an event).</t>
+  </si>
+  <si>
+    <t>Note: outer loop ends when there is no event to attend and there is no more available events in the schedule(number of events &lt; number of days). Endday is the priority.</t>
+  </si>
+  <si>
+    <t>Lexigraphical Comparison</t>
   </si>
 </sst>
 </file>
@@ -675,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1179,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>303</v>
       </c>
@@ -1181,7 +1196,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1865</v>
       </c>
@@ -1198,7 +1213,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>326</v>
       </c>
@@ -1210,6 +1225,26 @@
       </c>
       <c r="D35" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1353</v>
+      </c>
+      <c r="B36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maximum Number Of Events That Can Be Attended 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811E6547-C6C1-49D7-8C05-8BC38C6D2525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE797B-A5C0-43D3-A5A1-CAE3D9817A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="125">
   <si>
     <t>Id</t>
   </si>
@@ -391,6 +391,15 @@
   </si>
   <si>
     <t>is a Power of Two and bits are in even places n &gt; 0 &amp;&amp; (n &amp; (n - 1)) == 0 &amp;&amp; (n &amp; 0x55555555) != 0</t>
+  </si>
+  <si>
+    <t>Maximum Number of Events That Can Be Attended 2</t>
+  </si>
+  <si>
+    <t>Binary Search/Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Sort the events by ENDday, have an array of EndDays, store best result in a multi-dim array.</t>
   </si>
 </sst>
 </file>
@@ -708,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,6 +1306,20 @@
         <v>121</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1751</v>
+      </c>
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reschedule Meetings For Max Free Time 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE797B-A5C0-43D3-A5A1-CAE3D9817A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD29B34-6E69-40B3-BB64-7BACDF11A000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
   <si>
     <t>Id</t>
   </si>
@@ -400,6 +400,15 @@
   </si>
   <si>
     <t>Sort the events by ENDday, have an array of EndDays, store best result in a multi-dim array.</t>
+  </si>
+  <si>
+    <t>Reschedule Meetings for Maximum Free Time 1</t>
+  </si>
+  <si>
+    <t>Window Strategy</t>
+  </si>
+  <si>
+    <t>Collect all gaps[], build a window and slide it to find max free time, we rearrange k meetings merge k+1 gaps, the max size of a window is k+1</t>
   </si>
 </sst>
 </file>
@@ -717,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,6 +1329,20 @@
         <v>124</v>
       </c>
     </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3469</v>
+      </c>
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reschedule Meetings For Maximum Time 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD29B34-6E69-40B3-BB64-7BACDF11A000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF56EDFA-B083-42B8-905A-EBB12B9620AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="1245" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
   <si>
     <t>Id</t>
   </si>
@@ -409,16 +409,28 @@
   </si>
   <si>
     <t>Collect all gaps[], build a window and slide it to find max free time, we rearrange k meetings merge k+1 gaps, the max size of a window is k+1</t>
+  </si>
+  <si>
+    <t>Reschedule Meetings for Maximum Free Time 2</t>
+  </si>
+  <si>
+    <t>Collect all gaps[], find the max gap to the left/right of the current gap, consider if we can expand the gap or not at the current meeting either to the left or right.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -726,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1355,22 @@
         <v>127</v>
       </c>
     </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3440</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reverse String & Reverse Vowels.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF56EDFA-B083-42B8-905A-EBB12B9620AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8610368-C3A5-4281-B894-FABE3293BB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="1245" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="134">
   <si>
     <t>Id</t>
   </si>
@@ -415,6 +415,18 @@
   </si>
   <si>
     <t>Collect all gaps[], find the max gap to the left/right of the current gap, consider if we can expand the gap or not at the current meeting either to the left or right.</t>
+  </si>
+  <si>
+    <t>Reverse String</t>
+  </si>
+  <si>
+    <t>2 Pointers</t>
+  </si>
+  <si>
+    <t>Reverse Vowels of a String</t>
+  </si>
+  <si>
+    <t>2 Pointers/List&lt;int&gt;</t>
   </si>
 </sst>
 </file>
@@ -738,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,6 +1381,28 @@
         <v>129</v>
       </c>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>344</v>
+      </c>
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>345</v>
+      </c>
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Intersection of 2 Arrays.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8610368-C3A5-4281-B894-FABE3293BB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41982A90-9172-4E1A-B686-B863281123D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="1245" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="136">
   <si>
     <t>Id</t>
   </si>
@@ -427,6 +427,12 @@
   </si>
   <si>
     <t>2 Pointers/List&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>Intersection of two arrays</t>
+  </si>
+  <si>
+    <t>List, HashSet</t>
   </si>
 </sst>
 </file>
@@ -750,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,6 +1409,17 @@
         <v>133</v>
       </c>
     </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>349</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Convert Binary Number In A Linked List To Integer.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41982A90-9172-4E1A-B686-B863281123D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2331D1D3-77F9-43BC-9B87-5540C90D9692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="1245" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="138">
   <si>
     <t>Id</t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>List, HashSet</t>
+  </si>
+  <si>
+    <t>Convert Binary Number in a Linked List to Integer</t>
+  </si>
+  <si>
+    <t>Bitwise, Leftshift, OR</t>
   </si>
 </sst>
 </file>
@@ -756,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,6 +1426,17 @@
         <v>135</v>
       </c>
     </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1290</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Find The Maximum Length Of Valid Subsequence 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652B5885-2A29-4BF1-B494-43719F3F0675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0DAF8E-8578-4F66-B87E-5B600EA1305D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="1245" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8775" yWindow="375" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
   <si>
     <t>Id</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>Valid Word</t>
+  </si>
+  <si>
+    <t>Find the Maximum Length of Valid Subsequent 1</t>
+  </si>
+  <si>
+    <t>Even/Odd, Dynamic Programming</t>
+  </si>
+  <si>
+    <t>(E+E)/2 = E; (O+O)/2 = E | (E+O)/2=O; (O+E)/2=O. Find the longest subsequence of evens, odds, e-o or o-e. Have a dp to keep track and compare foreach element</t>
   </si>
 </sst>
 </file>
@@ -765,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,6 +1457,20 @@
         <v>138</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3201</v>
+      </c>
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Intersection Of Two Arrays 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0DAF8E-8578-4F66-B87E-5B600EA1305D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537FC4FC-7B89-4DC1-AE69-E3087B55FD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8775" yWindow="375" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
   <si>
     <t>Id</t>
   </si>
@@ -451,6 +451,18 @@
   </si>
   <si>
     <t>(E+E)/2 = E; (O+O)/2 = E | (E+O)/2=O; (O+E)/2=O. Find the longest subsequence of evens, odds, e-o or o-e. Have a dp to keep track and compare foreach element</t>
+  </si>
+  <si>
+    <t>Intersection of two arrays 2</t>
+  </si>
+  <si>
+    <t>Dictionary/Sorting/Skipping</t>
+  </si>
+  <si>
+    <t>Valid Perfect Square</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
   </si>
 </sst>
 </file>
@@ -774,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,6 +1483,28 @@
         <v>141</v>
       </c>
     </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>350</v>
+      </c>
+      <c r="B48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>367</v>
+      </c>
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Guess Number Higher Or Lower.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537FC4FC-7B89-4DC1-AE69-E3087B55FD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6986008A-422D-4E9A-BBC5-D744834924D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8775" yWindow="375" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="147">
   <si>
     <t>Id</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Guess Number Higher or Lower</t>
   </si>
 </sst>
 </file>
@@ -786,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,6 +1508,17 @@
         <v>145</v>
       </c>
     </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>374</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First Unique Character In A String.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C1BC4-512B-4D3E-AB07-A81D34492A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49AC04B-5B78-4456-8711-689EDC74B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8925" yWindow="1020" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
   <si>
     <t>Id</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>Dictionary/HashMap/Array[26]</t>
+  </si>
+  <si>
+    <t>First Unique Character In A String</t>
   </si>
 </sst>
 </file>
@@ -795,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,6 +1539,17 @@
         <v>148</v>
       </c>
     </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>387</v>
+      </c>
+      <c r="B52" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove Subfolders From The Filesystem.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49AC04B-5B78-4456-8711-689EDC74B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD27527D-DC73-4BD3-B04F-78E2F3EC0BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8925" yWindow="1020" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
   <si>
     <t>Id</t>
   </si>
@@ -475,6 +475,15 @@
   </si>
   <si>
     <t>First Unique Character In A String</t>
+  </si>
+  <si>
+    <t>Remove Sub-Folders from the Filesystem</t>
+  </si>
+  <si>
+    <t>Sorting lexicographically</t>
+  </si>
+  <si>
+    <t>Sort then loop path.StartsWith</t>
   </si>
 </sst>
 </file>
@@ -798,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1515,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>367</v>
       </c>
@@ -1517,7 +1526,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>374</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>383</v>
       </c>
@@ -1539,7 +1548,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>387</v>
       </c>
@@ -1548,6 +1557,20 @@
       </c>
       <c r="C52" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1233</v>
+      </c>
+      <c r="B53" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete Duplicate Folders In System.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0F3AD-8014-442F-BFA3-A510D2D01494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBFE8D9-8216-4160-90E2-1B996CB91CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="157">
   <si>
     <t>Id</t>
   </si>
@@ -487,6 +487,15 @@
   </si>
   <si>
     <t>Find The Difference</t>
+  </si>
+  <si>
+    <t>Delete Duplicate Folders in System</t>
+  </si>
+  <si>
+    <t>Trie</t>
+  </si>
+  <si>
+    <t>Make a private class: name, subfolders, serial -&gt; Build a Trie -&gt; Post Order to Serialize -&gt; Postorder to Mark Delete -&gt; Preorder to collect</t>
   </si>
 </sst>
 </file>
@@ -810,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,6 +1596,20 @@
         <v>127</v>
       </c>
     </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1948</v>
+      </c>
+      <c r="B55" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Delete Characters To Make Fancy String.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248B8EBD-7973-495D-8E95-A4A35BAFEF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D344F24B-EAE9-4FC7-8B53-F981B8E7993C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8925" yWindow="1020" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="161">
   <si>
     <t>Id</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>Delete Characters To Make Fancy String</t>
+  </si>
+  <si>
+    <t>1 Pointer/Count</t>
+  </si>
+  <si>
+    <t>Iterate, count and skip</t>
   </si>
 </sst>
 </file>
@@ -827,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,6 +1640,12 @@
       <c r="B57" t="s">
         <v>158</v>
       </c>
+      <c r="C57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">

</xml_diff>

<commit_message>
Sum Of Left Leaves.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D344F24B-EAE9-4FC7-8B53-F981B8E7993C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE9409-3C91-48C3-BFA5-C199E98AAE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8925" yWindow="1020" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="163">
   <si>
     <t>Id</t>
   </si>
@@ -508,6 +508,12 @@
   </si>
   <si>
     <t>Iterate, count and skip</t>
+  </si>
+  <si>
+    <t>Sum of Left Leaves</t>
+  </si>
+  <si>
+    <t>Recursive</t>
   </si>
 </sst>
 </file>
@@ -831,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,6 +1653,17 @@
         <v>160</v>
       </c>
     </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>404</v>
+      </c>
+      <c r="B58" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximum Unique Subarray Sum After Deletion.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31695AB5-4A0F-4EEE-92E0-C5F355C065C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6426EE-C43A-4B55-8BAE-0332E15B5B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="169">
   <si>
     <t>Id</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>Have a HashSet&lt;int&gt; for seen, moving to the right, if the element is in seen, shrink from the left, keep track of the maximum of current sum</t>
+  </si>
+  <si>
+    <t>Maximum Unique Subarray Sum After Deletion</t>
+  </si>
+  <si>
+    <t>HashSet/Max/Array of Uniques</t>
+  </si>
+  <si>
+    <t>Have a hashSet&lt;int&gt; Or int[] map to store the unique elements, have a variable max, if max &lt; 0 return max, else return sum of uniques</t>
   </si>
 </sst>
 </file>
@@ -846,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,6 +1696,20 @@
         <v>165</v>
       </c>
     </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>3487</v>
+      </c>
+      <c r="B60" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Convert a number to Hexadecimal.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D61801-A3F3-4CA6-9988-6AF4512307D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDFCC96-1E92-4345-BA18-4B6493972052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="175">
   <si>
     <t>Id</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>Count Bits by &amp; and shift or, x = x &amp; (x-1). Nested loop to check all possible time, add to the result with valid string</t>
+  </si>
+  <si>
+    <t>Convert A Number to Hexadecimal</t>
+  </si>
+  <si>
+    <t>Bitwise/Math/Uint</t>
+  </si>
+  <si>
+    <t>cast to uint, do /16 or &gt;&gt;4</t>
   </si>
 </sst>
 </file>
@@ -864,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,6 +1742,20 @@
         <v>171</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>405</v>
+      </c>
+      <c r="B62" t="s">
+        <v>172</v>
+      </c>
+      <c r="C62" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Convert Integer to the Sum of Two No-Zero Integers.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAD67EB-37D9-439C-B60D-936DAC377D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5D3625-FFD8-4877-901E-59BFBEE67618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7770" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="181">
   <si>
     <t>Id</t>
   </si>
@@ -561,7 +561,13 @@
     <t>Fizz Buzz</t>
   </si>
   <si>
-    <t>If-else/Switch-case</t>
+    <t>If-else/Switch-case/ Use flag = (i % 3 == 0) + 2 * (i % 5 == 0);</t>
+  </si>
+  <si>
+    <t>Fruits Into Baskets 2</t>
+  </si>
+  <si>
+    <t>Largest 3-Same-Digit Number in a String</t>
   </si>
 </sst>
 </file>
@@ -885,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,6 +1802,22 @@
         <v>178</v>
       </c>
     </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>3477</v>
+      </c>
+      <c r="B65" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2264</v>
+      </c>
+      <c r="B66" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Fruits Into Basket 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5D3625-FFD8-4877-901E-59BFBEE67618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8E653D-9051-4EF0-9B24-64FE3AE7BB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="186">
   <si>
     <t>Id</t>
   </si>
@@ -568,6 +571,21 @@
   </si>
   <si>
     <t>Largest 3-Same-Digit Number in a String</t>
+  </si>
+  <si>
+    <t>Convert Integers to the Sum of Two No-Zero Integers</t>
+  </si>
+  <si>
+    <t>Use a util function to check a zero in the digits/Loop until both number have no zero</t>
+  </si>
+  <si>
+    <t>Iteration/Loop</t>
+  </si>
+  <si>
+    <t>Loop in Loop</t>
+  </si>
+  <si>
+    <t>Can use a track for usedBasket</t>
   </si>
 </sst>
 </file>
@@ -891,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,20 +1820,43 @@
         <v>178</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3477</v>
       </c>
       <c r="B65" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>183</v>
+      </c>
+      <c r="D65" t="s">
+        <v>184</v>
+      </c>
+      <c r="E65" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2264</v>
       </c>
       <c r="B66" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1317</v>
+      </c>
+      <c r="B67" t="s">
+        <v>181</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Largest 3 Same Digit Number in String.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8E653D-9051-4EF0-9B24-64FE3AE7BB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791CCD3D-FA1B-4891-923F-7EB70AA6C393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="191">
   <si>
     <t>Id</t>
   </si>
@@ -586,6 +586,21 @@
   </si>
   <si>
     <t>Can use a track for usedBasket</t>
+  </si>
+  <si>
+    <t>Create HelloWorld Function</t>
+  </si>
+  <si>
+    <t>TypeScript</t>
+  </si>
+  <si>
+    <t>return "Hello World"</t>
+  </si>
+  <si>
+    <t>List/Loop</t>
+  </si>
+  <si>
+    <t>C# Contains</t>
   </si>
 </sst>
 </file>
@@ -909,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,6 +1859,12 @@
       <c r="B66" t="s">
         <v>180</v>
       </c>
+      <c r="C66" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
@@ -1857,6 +1878,20 @@
       </c>
       <c r="D67" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2667</v>
+      </c>
+      <c r="B68" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" t="s">
+        <v>187</v>
+      </c>
+      <c r="D68" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sort Vowels In A String.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791CCD3D-FA1B-4891-923F-7EB70AA6C393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA31C94D-059F-4484-AAEC-EBA1714D25C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="194">
   <si>
     <t>Id</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>C# Contains</t>
+  </si>
+  <si>
+    <t>Sort Vowels In A String</t>
+  </si>
+  <si>
+    <t>Array/2 Pointers</t>
+  </si>
+  <si>
+    <t>C#: Array of vowels, Array of s, Collect the vowels, Sort the vowels, replace the vowels in s with the sorted vowels</t>
   </si>
 </sst>
 </file>
@@ -924,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,6 +1903,20 @@
         <v>188</v>
       </c>
     </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2785</v>
+      </c>
+      <c r="B69" t="s">
+        <v>191</v>
+      </c>
+      <c r="C69" t="s">
+        <v>192</v>
+      </c>
+      <c r="D69" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Average Salary Excluding The Min And Max Salary.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA31C94D-059F-4484-AAEC-EBA1714D25C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09B37FD-9F78-42D5-847B-76DFF743DF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="198">
   <si>
     <t>Id</t>
   </si>
@@ -610,6 +610,18 @@
   </si>
   <si>
     <t>C#: Array of vowels, Array of s, Collect the vowels, Sort the vowels, replace the vowels in s with the sorted vowels</t>
+  </si>
+  <si>
+    <t>C++: vector, std::sort, string.fin(c) != std::string::npos</t>
+  </si>
+  <si>
+    <t>Average Salary Excluding the Min and Max Salaray</t>
+  </si>
+  <si>
+    <t>Minimum Number of People to Teach</t>
+  </si>
+  <si>
+    <t>3 Pointers/Math</t>
   </si>
 </sst>
 </file>
@@ -933,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,6 +1928,28 @@
       <c r="D69" t="s">
         <v>193</v>
       </c>
+      <c r="E69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1491</v>
+      </c>
+      <c r="B70" t="s">
+        <v>195</v>
+      </c>
+      <c r="C70" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1733</v>
+      </c>
+      <c r="B71" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">

</xml_diff>

<commit_message>
Maximum Number of Words Can Be Typed
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09B37FD-9F78-42D5-847B-76DFF743DF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10383DF-BDEA-42FD-A66E-7AE4B02A7D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="1575" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="202">
   <si>
     <t>Id</t>
   </si>
@@ -612,9 +612,6 @@
     <t>C#: Array of vowels, Array of s, Collect the vowels, Sort the vowels, replace the vowels in s with the sorted vowels</t>
   </si>
   <si>
-    <t>C++: vector, std::sort, string.fin(c) != std::string::npos</t>
-  </si>
-  <si>
     <t>Average Salary Excluding the Min and Max Salaray</t>
   </si>
   <si>
@@ -622,6 +619,21 @@
   </si>
   <si>
     <t>3 Pointers/Math</t>
+  </si>
+  <si>
+    <t>Vowels Game in a String</t>
+  </si>
+  <si>
+    <t>Maximum Number of Words You Can Type</t>
+  </si>
+  <si>
+    <t>Loop/String manipulation</t>
+  </si>
+  <si>
+    <t>C++: vector, std::sort, string.find(c) != std::string::npos</t>
+  </si>
+  <si>
+    <t>string stream &gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -945,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1941,7 @@
         <v>193</v>
       </c>
       <c r="E69" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,10 +1949,10 @@
         <v>1491</v>
       </c>
       <c r="B70" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1948,7 +1960,32 @@
         <v>1733</v>
       </c>
       <c r="B71" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>3227</v>
+      </c>
+      <c r="B72" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1935</v>
+      </c>
+      <c r="B73" t="s">
+        <v>198</v>
+      </c>
+      <c r="C73" t="s">
+        <v>199</v>
+      </c>
+      <c r="D73" t="s">
+        <v>184</v>
+      </c>
+      <c r="E73" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Count Elements With Maximum Frequencies.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10383DF-BDEA-42FD-A66E-7AE4B02A7D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6204952F-7AD0-40B4-A7FA-967DB6223CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="1575" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8910" yWindow="1695" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="205">
   <si>
     <t>Id</t>
   </si>
@@ -634,6 +634,15 @@
   </si>
   <si>
     <t>string stream &gt;&gt;</t>
+  </si>
+  <si>
+    <t>Count Elements With Maximum Frequency</t>
+  </si>
+  <si>
+    <t>Dictionary/Unordered_map</t>
+  </si>
+  <si>
+    <t>Count frequencies of each element, find the max, add the sum of max frequency</t>
   </si>
 </sst>
 </file>
@@ -957,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,6 +1997,20 @@
         <v>201</v>
       </c>
     </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>3005</v>
+      </c>
+      <c r="B74" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" t="s">
+        <v>203</v>
+      </c>
+      <c r="D74" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Adjacent Increasing Subarrays Detection I.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6204952F-7AD0-40B4-A7FA-967DB6223CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE4428-E6A6-4D6F-AA92-F0B7E4AF6212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8910" yWindow="1695" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="208">
   <si>
     <t>Id</t>
   </si>
@@ -643,6 +643,15 @@
   </si>
   <si>
     <t>Count frequencies of each element, find the max, add the sum of max frequency</t>
+  </si>
+  <si>
+    <t>Adjacent Increasing Subarrays Detection I</t>
+  </si>
+  <si>
+    <t>Loop/ Helper function</t>
+  </si>
+  <si>
+    <t>Use a helper function to check strictly increasing segment, loop each element to check the 2 adjacent segments</t>
   </si>
 </sst>
 </file>
@@ -966,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,6 +2020,20 @@
         <v>204</v>
       </c>
     </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3349</v>
+      </c>
+      <c r="B75" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Vowels Game In A String.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE4428-E6A6-4D6F-AA92-F0B7E4AF6212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E6160-CF3F-4719-971C-3C4EEF7493DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="210">
   <si>
     <t>Id</t>
   </si>
@@ -652,6 +652,12 @@
   </si>
   <si>
     <t>Use a helper function to check strictly increasing segment, loop each element to check the 2 adjacent segments</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>Check and count vowels, 0 Bob wins, otherwise Alice wins</t>
   </si>
 </sst>
 </file>
@@ -977,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,6 +1994,12 @@
       <c r="B72" t="s">
         <v>197</v>
       </c>
+      <c r="C72" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">

</xml_diff>

<commit_message>
Smallest Missing Non Negative Integer After Operations.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E6160-CF3F-4719-971C-3C4EEF7493DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC880F3-A4F9-496B-8801-DF95E370AB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="213">
   <si>
     <t>Id</t>
   </si>
@@ -658,6 +658,15 @@
   </si>
   <si>
     <t>Check and count vowels, 0 Bob wins, otherwise Alice wins</t>
+  </si>
+  <si>
+    <t>Smallest Missing Non-negative Integer after Operations</t>
+  </si>
+  <si>
+    <t>Dictionary/ Loop</t>
+  </si>
+  <si>
+    <t>Collect a freq table for remainders of each element / value. Exhaust the increasing mex in the freq table</t>
   </si>
 </sst>
 </file>
@@ -981,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,6 +2055,20 @@
         <v>207</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2598</v>
+      </c>
+      <c r="B76" t="s">
+        <v>210</v>
+      </c>
+      <c r="C76" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Final Value Of Variable After Performing Operations.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC880F3-A4F9-496B-8801-DF95E370AB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397EF73F-11DC-4A68-855F-DEDB9D5DD770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="215">
   <si>
     <t>Id</t>
   </si>
@@ -667,6 +667,12 @@
   </si>
   <si>
     <t>Collect a freq table for remainders of each element / value. Exhaust the increasing mex in the freq table</t>
+  </si>
+  <si>
+    <t>Final Value of Variable After Performing Operations</t>
+  </si>
+  <si>
+    <t>C# contains</t>
   </si>
 </sst>
 </file>
@@ -990,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,6 +2075,20 @@
         <v>212</v>
       </c>
     </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2011</v>
+      </c>
+      <c r="B77" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Check If Digits Are Equal In String AFter Operations 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397EF73F-11DC-4A68-855F-DEDB9D5DD770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E31BFE-9034-481E-98C3-4E40D016AA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="217">
   <si>
     <t>Id</t>
   </si>
@@ -673,6 +673,12 @@
   </si>
   <si>
     <t>C# contains</t>
+  </si>
+  <si>
+    <t>Check If Digits Are Equal in String Operations 1</t>
+  </si>
+  <si>
+    <t>C# StringBuilder for tracking new numbers</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
       <selection activeCell="D78" sqref="D78"/>
@@ -2089,6 +2095,20 @@
         <v>214</v>
       </c>
     </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>3461</v>
+      </c>
+      <c r="B78" t="s">
+        <v>215</v>
+      </c>
+      <c r="C78" t="s">
+        <v>208</v>
+      </c>
+      <c r="D78" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Next Greater Numerically Balanced Number.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E31BFE-9034-481E-98C3-4E40D016AA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BFB383-EA88-4744-B2FC-F7938B3FE267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="218">
   <si>
     <t>Id</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>C# StringBuilder for tracking new numbers</t>
+  </si>
+  <si>
+    <t>C++ string.erase(string.size() - 1)</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2111,9 @@
       <c r="D78" t="s">
         <v>216</v>
       </c>
+      <c r="E78" t="s">
+        <v>217</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">

</xml_diff>

<commit_message>
Number Of Laser Beams In A Bank.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BFB383-EA88-4744-B2FC-F7938B3FE267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F17F510-1737-45C2-8ADF-9AB8E2512DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="223">
   <si>
     <t>Id</t>
   </si>
@@ -682,6 +682,21 @@
   </si>
   <si>
     <t>C++ string.erase(string.size() - 1)</t>
+  </si>
+  <si>
+    <t>Next Greater Numerically Balanced Number</t>
+  </si>
+  <si>
+    <t>Constraint is 10^6, max possible balanced number is 1224444, iterate upto max and check each</t>
+  </si>
+  <si>
+    <t>Number of Laser Beams in a Bank</t>
+  </si>
+  <si>
+    <t>Loop/Math</t>
+  </si>
+  <si>
+    <t>Count devices in each row, multiply with the next available row and add them to the sum</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,6 +2130,34 @@
         <v>217</v>
       </c>
     </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2048</v>
+      </c>
+      <c r="B79" t="s">
+        <v>218</v>
+      </c>
+      <c r="C79" t="s">
+        <v>75</v>
+      </c>
+      <c r="D79" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2125</v>
+      </c>
+      <c r="B80" t="s">
+        <v>220</v>
+      </c>
+      <c r="C80" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Make Array Elements Equal To Zero.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F17F510-1737-45C2-8ADF-9AB8E2512DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2CEEC3-6E51-4271-867B-7B7ADCD41064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="225">
   <si>
     <t>Id</t>
   </si>
@@ -697,6 +697,12 @@
   </si>
   <si>
     <t>Count devices in each row, multiply with the next available row and add them to the sum</t>
+  </si>
+  <si>
+    <t>Make Array Elements Equal to Zero</t>
+  </si>
+  <si>
+    <t>Clone the Array, Make a helper function and simulate the process</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,6 +2164,20 @@
         <v>222</v>
       </c>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>3354</v>
+      </c>
+      <c r="B81" t="s">
+        <v>223</v>
+      </c>
+      <c r="C81" t="s">
+        <v>221</v>
+      </c>
+      <c r="D81" t="s">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Number Of Increments On Subarray ToF  rm A Target Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2CEEC3-6E51-4271-867B-7B7ADCD41064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E660BF13-53B2-4BE8-8CF3-21DB750BE376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="1860" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4590" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="228">
   <si>
     <t>Id</t>
   </si>
@@ -703,6 +703,15 @@
   </si>
   <si>
     <t>Clone the Array, Make a helper function and simulate the process</t>
+  </si>
+  <si>
+    <t>Smallest Number With All Set Bits</t>
+  </si>
+  <si>
+    <t>Power of 2 minus 1</t>
+  </si>
+  <si>
+    <t>Minimum Number of Increments on Subarrays to Form a Target Array</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,6 +2187,31 @@
         <v>224</v>
       </c>
     </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>3370</v>
+      </c>
+      <c r="B82" t="s">
+        <v>225</v>
+      </c>
+      <c r="C82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1526</v>
+      </c>
+      <c r="B83" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
The Two Sneaky Numbers Of Digitville.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E660BF13-53B2-4BE8-8CF3-21DB750BE376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16617335-3AD5-46C1-9CA7-4FAF2FF76FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="4590" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="229">
   <si>
     <t>Id</t>
   </si>
@@ -712,6 +712,9 @@
   </si>
   <si>
     <t>Minimum Number of Increments on Subarrays to Form a Target Array</t>
+  </si>
+  <si>
+    <t>The Two Sneaky Numbers of Digitville</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2212,6 +2215,17 @@
         <v>97</v>
       </c>
     </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>3289</v>
+      </c>
+      <c r="B84" t="s">
+        <v>228</v>
+      </c>
+      <c r="C84" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Delete Nodes From Linked List Present in Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16617335-3AD5-46C1-9CA7-4FAF2FF76FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C5F6BC-4A22-4F94-9B0E-2B9857C86A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6645" yWindow="4410" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="232">
   <si>
     <t>Id</t>
   </si>
@@ -715,6 +715,15 @@
   </si>
   <si>
     <t>The Two Sneaky Numbers of Digitville</t>
+  </si>
+  <si>
+    <t>Delete Nodes From Linked List Present in Array</t>
+  </si>
+  <si>
+    <t>HashSet/Loop</t>
+  </si>
+  <si>
+    <t>Have a hash set for faster look up, skipping to find the head, then skipping to delete nodes</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,6 +2235,20 @@
         <v>221</v>
       </c>
     </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>3217</v>
+      </c>
+      <c r="B85" t="s">
+        <v>229</v>
+      </c>
+      <c r="C85" t="s">
+        <v>230</v>
+      </c>
+      <c r="D85" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Unguarded Cells In the Grid.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C5F6BC-4A22-4F94-9B0E-2B9857C86A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B91E70B-0570-486F-AE81-3ACE2BB07804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="4410" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6645" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="235">
   <si>
     <t>Id</t>
   </si>
@@ -724,6 +724,15 @@
   </si>
   <si>
     <t>Have a hash set for faster look up, skipping to find the head, then skipping to delete nodes</t>
+  </si>
+  <si>
+    <t>Count Unguarded Cells in the Grid</t>
+  </si>
+  <si>
+    <t>Loop/2D Array</t>
+  </si>
+  <si>
+    <t>Place G and W, iteration over 4 directions</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,6 +2258,20 @@
         <v>231</v>
       </c>
     </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2257</v>
+      </c>
+      <c r="B86" t="s">
+        <v>232</v>
+      </c>
+      <c r="C86" t="s">
+        <v>233</v>
+      </c>
+      <c r="D86" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Time To Make Rope Colorful.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B91E70B-0570-486F-AE81-3ACE2BB07804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1FFB2D-3227-4978-9E82-34537AE5D98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="3510" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="238">
   <si>
     <t>Id</t>
   </si>
@@ -733,6 +733,15 @@
   </si>
   <si>
     <t>Place G and W, iteration over 4 directions</t>
+  </si>
+  <si>
+    <t>Minimum Time To Make Rope Colorful</t>
+  </si>
+  <si>
+    <t>Loop/Skip/Math</t>
+  </si>
+  <si>
+    <t>Loop, keep a running sum, find a max, forward the max</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1065,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
       <selection activeCell="D87" sqref="D87"/>
@@ -2272,6 +2281,20 @@
         <v>234</v>
       </c>
     </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1578</v>
+      </c>
+      <c r="B87" t="s">
+        <v>235</v>
+      </c>
+      <c r="C87" t="s">
+        <v>236</v>
+      </c>
+      <c r="D87" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Find X-Sum of All K-Long Subarray 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1FFB2D-3227-4978-9E82-34537AE5D98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97789D74-B529-46A8-A1E4-0B03AFD543FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3510" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="243">
   <si>
     <t>Id</t>
   </si>
@@ -742,6 +742,21 @@
   </si>
   <si>
     <t>Loop, keep a running sum, find a max, forward the max</t>
+  </si>
+  <si>
+    <t>Compare 2 consecutive elements, forward the bigger value if it's first</t>
+  </si>
+  <si>
+    <t>Find X-Sum of All K-Long Subarray 1</t>
+  </si>
+  <si>
+    <t>Loop/Math/Helper Function</t>
+  </si>
+  <si>
+    <t>Sliding window, frequency table, LinQ</t>
+  </si>
+  <si>
+    <t>freq.Sort((a, b) =&gt; b[0] != a[0] ? b[0] - a[0] : b[1] - a[1])</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="E64" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,7 +2218,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3354</v>
       </c>
@@ -2217,7 +2232,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>3370</v>
       </c>
@@ -2231,7 +2246,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1526</v>
       </c>
@@ -2242,7 +2257,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3289</v>
       </c>
@@ -2253,7 +2268,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3217</v>
       </c>
@@ -2267,7 +2282,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2257</v>
       </c>
@@ -2281,7 +2296,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1578</v>
       </c>
@@ -2293,6 +2308,26 @@
       </c>
       <c r="D87" t="s">
         <v>237</v>
+      </c>
+      <c r="E87" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>3318</v>
+      </c>
+      <c r="B88" t="s">
+        <v>239</v>
+      </c>
+      <c r="C88" t="s">
+        <v>240</v>
+      </c>
+      <c r="D88" t="s">
+        <v>241</v>
+      </c>
+      <c r="E88" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minimum One Bit Operations To Make Integers Zero.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97789D74-B529-46A8-A1E4-0B03AFD543FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00821092-DA08-42F9-B9B4-697D070C4445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="246">
   <si>
     <t>Id</t>
   </si>
@@ -757,6 +757,15 @@
   </si>
   <si>
     <t>freq.Sort((a, b) =&gt; b[0] != a[0] ? b[0] - a[0] : b[1] - a[1])</t>
+  </si>
+  <si>
+    <t>Minimum One Bit Operations To Make Integers Zero</t>
+  </si>
+  <si>
+    <t>Bitwise</t>
+  </si>
+  <si>
+    <t>Gray Code</t>
   </si>
 </sst>
 </file>
@@ -1080,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E64" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,6 +2339,20 @@
         <v>242</v>
       </c>
     </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1611</v>
+      </c>
+      <c r="B89" t="s">
+        <v>243</v>
+      </c>
+      <c r="C89" t="s">
+        <v>244</v>
+      </c>
+      <c r="D89" t="s">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Operations To Obtain Zero.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00821092-DA08-42F9-B9B4-697D070C4445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057FCF1C-2CBF-49C5-8140-88BB32D8A0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
   <si>
     <t>Id</t>
   </si>
@@ -766,6 +766,12 @@
   </si>
   <si>
     <t>Gray Code</t>
+  </si>
+  <si>
+    <t>Count Operations to Obtain Zero</t>
+  </si>
+  <si>
+    <t>Simulate the process or Eucludean algorithm</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,6 +2359,20 @@
         <v>245</v>
       </c>
     </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2169</v>
+      </c>
+      <c r="B90" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Operations To Convert All Elements To Zero.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057FCF1C-2CBF-49C5-8140-88BB32D8A0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5DD916-D4E7-4C8D-B69F-CC1AECCD4EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="251">
   <si>
     <t>Id</t>
   </si>
@@ -772,6 +772,15 @@
   </si>
   <si>
     <t>Simulate the process or Eucludean algorithm</t>
+  </si>
+  <si>
+    <t>Minimum Operations To Convert All Elements To Zero</t>
+  </si>
+  <si>
+    <t>Loop/Stack</t>
+  </si>
+  <si>
+    <t>Have a stack sentinel 0, loop each num, if num == 0, we empty out the stack. While num &lt; stack.Peek(), we pop the stack until they're equal and that would be the current other end of the array. If num &gt; stack.Peek(), we need a new ops and push the num in the stack.</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,6 +2382,20 @@
         <v>247</v>
       </c>
     </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>3542</v>
+      </c>
+      <c r="B91" t="s">
+        <v>248</v>
+      </c>
+      <c r="C91" t="s">
+        <v>249</v>
+      </c>
+      <c r="D91" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum of Operations To Make All Array Elements Equal to 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1E6DA7-423D-4619-AE6F-4BF057329005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EB4EBA-92A0-4AAB-A1F3-0315B7F37F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="256">
   <si>
     <t>Id</t>
   </si>
@@ -790,6 +790,12 @@
   </si>
   <si>
     <t>Each string count zeroes and ones, DP update reverse to pick or skip</t>
+  </si>
+  <si>
+    <t>Minimum of Operations To Make All Array Elements Equal to 1</t>
+  </si>
+  <si>
+    <t>Helper function to find GCD. 1/ If GCD of all elements &gt; 1, return -1. 2/ If there is a one, return nums.Length - ones. 3/ Loop in Loop to find the shortest subarray that has GCD 1, return n + shortest.Length() - 2</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,11 +2425,26 @@
         <v>253</v>
       </c>
     </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2654</v>
+      </c>
+      <c r="B93" t="s">
+        <v>254</v>
+      </c>
+      <c r="C93" t="s">
+        <v>75</v>
+      </c>
+      <c r="D93" t="s">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Maximum Number of Operations To Move Ones to the End.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EB4EBA-92A0-4AAB-A1F3-0315B7F37F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB4BCCC-9777-4471-8966-1638601591AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="258">
   <si>
     <t>Id</t>
   </si>
@@ -796,6 +796,12 @@
   </si>
   <si>
     <t>Helper function to find GCD. 1/ If GCD of all elements &gt; 1, return -1. 2/ If there is a one, return nums.Length - ones. 3/ Loop in Loop to find the shortest subarray that has GCD 1, return n + shortest.Length() - 2</t>
+  </si>
+  <si>
+    <t>Maximum Number of Operations To Move Ones to the End</t>
+  </si>
+  <si>
+    <t>Every '0' will pass by '1' to the left of it, group of consecutive '0's is counted as one '0' because '1' can slide through them.</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,6 +2445,20 @@
         <v>255</v>
       </c>
     </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>3228</v>
+      </c>
+      <c r="B94" t="s">
+        <v>256</v>
+      </c>
+      <c r="C94" t="s">
+        <v>75</v>
+      </c>
+      <c r="D94" t="s">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Increment Submatrices By One.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB4BCCC-9777-4471-8966-1638601591AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A50125-EF6D-4F30-BC78-4D62A1680F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="261">
   <si>
     <t>Id</t>
   </si>
@@ -802,6 +802,15 @@
   </si>
   <si>
     <t>Every '0' will pass by '1' to the left of it, group of consecutive '0's is counted as one '0' because '1' can slide through them.</t>
+  </si>
+  <si>
+    <t>Increment Submatrices By One</t>
+  </si>
+  <si>
+    <t>Cool Flag Array (Helper Array/Diff Array) to flag the prefix sum</t>
+  </si>
+  <si>
+    <t>flag[r1][c1] += 1; flag[r1][c2 + 1] -= 1; flag[r2 + 1][c1] -= 1; flag[r2 + 1][c2 + 1] += 1;</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2459,6 +2468,23 @@
         <v>257</v>
       </c>
     </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2536</v>
+      </c>
+      <c r="B95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C95" t="s">
+        <v>75</v>
+      </c>
+      <c r="D95" t="s">
+        <v>259</v>
+      </c>
+      <c r="E95" t="s">
+        <v>260</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count the Number of Substrings With Dominant Ones.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A50125-EF6D-4F30-BC78-4D62A1680F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637FC67-EE45-48F1-9153-EBCE6AD516AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="264">
   <si>
     <t>Id</t>
   </si>
@@ -811,6 +811,15 @@
   </si>
   <si>
     <t>flag[r1][c1] += 1; flag[r1][c2 + 1] -= 1; flag[r2 + 1][c1] -= 1; flag[r2 + 1][c2 + 1] += 1;</t>
+  </si>
+  <si>
+    <t>Count the Number of Substrings With Dominant Ones</t>
+  </si>
+  <si>
+    <t>Number of Substrings With Only 1s</t>
+  </si>
+  <si>
+    <t>Triangular Number, sum of sequence of 1s ( 1,2,3,…,n) = n(n+1)/2</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,6 +2494,31 @@
         <v>260</v>
       </c>
     </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>3234</v>
+      </c>
+      <c r="B96" t="s">
+        <v>261</v>
+      </c>
+      <c r="C96" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1513</v>
+      </c>
+      <c r="B97" t="s">
+        <v>262</v>
+      </c>
+      <c r="C97" t="s">
+        <v>75</v>
+      </c>
+      <c r="D97" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Number of Substrings With Only 1s.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637FC67-EE45-48F1-9153-EBCE6AD516AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B204B1-F04D-46E6-9D31-22D3E69A5C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="265">
   <si>
     <t>Id</t>
   </si>
@@ -819,7 +819,10 @@
     <t>Number of Substrings With Only 1s</t>
   </si>
   <si>
-    <t>Triangular Number, sum of sequence of 1s ( 1,2,3,…,n) = n(n+1)/2</t>
+    <t>Warning, can exceed 64-bit int (type long limit).</t>
+  </si>
+  <si>
+    <t>Triangular Number, sum of sequence of 1s ( 1,2,3,…,n) = n(n+1)/2. Can also have a Map/Dictionary to store groups of 1s and compute Key * Value</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D79" workbookViewId="0">
       <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
@@ -2505,7 +2508,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1513</v>
       </c>
@@ -2516,6 +2519,9 @@
         <v>75</v>
       </c>
       <c r="D97" t="s">
+        <v>264</v>
+      </c>
+      <c r="E97" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Check If All 1s Are At Least Length K Places Away.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B204B1-F04D-46E6-9D31-22D3E69A5C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3681D7-7BA2-4495-B71A-DA22B9417DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="268">
   <si>
     <t>Id</t>
   </si>
@@ -823,6 +823,15 @@
   </si>
   <si>
     <t>Triangular Number, sum of sequence of 1s ( 1,2,3,…,n) = n(n+1)/2. Can also have a Map/Dictionary to store groups of 1s and compute Key * Value</t>
+  </si>
+  <si>
+    <t>Check If All 1's Are at Least Length K Places Away</t>
+  </si>
+  <si>
+    <t>Loop/List</t>
+  </si>
+  <si>
+    <t>Loop, if 1, compute distance, check</t>
   </si>
 </sst>
 </file>
@@ -1146,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D79" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,6 +2534,20 @@
         <v>263</v>
       </c>
     </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1437</v>
+      </c>
+      <c r="B98" t="s">
+        <v>265</v>
+      </c>
+      <c r="C98" t="s">
+        <v>266</v>
+      </c>
+      <c r="D98" t="s">
+        <v>267</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
1-bit and 2-bit Characters.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3681D7-7BA2-4495-B71A-DA22B9417DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221A9F89-8292-4DC2-B3AA-1E5FFD246B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="271">
   <si>
     <t>Id</t>
   </si>
@@ -832,6 +832,15 @@
   </si>
   <si>
     <t>Loop, if 1, compute distance, check</t>
+  </si>
+  <si>
+    <t>1-bit and 2-bit Characters</t>
+  </si>
+  <si>
+    <t>Loop/Skip</t>
+  </si>
+  <si>
+    <t>Loop if 0, i++; else i+=2</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,6 +2557,20 @@
         <v>267</v>
       </c>
     </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>717</v>
+      </c>
+      <c r="B99" t="s">
+        <v>268</v>
+      </c>
+      <c r="C99" t="s">
+        <v>269</v>
+      </c>
+      <c r="D99" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Keep Multiplying Found Values By Two.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221A9F89-8292-4DC2-B3AA-1E5FFD246B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B89E53-2328-497C-93A6-8106ED42BCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="274">
   <si>
     <t>Id</t>
   </si>
@@ -841,6 +841,15 @@
   </si>
   <si>
     <t>Loop if 0, i++; else i+=2</t>
+  </si>
+  <si>
+    <t>Keep Multiplying Found Values By Two</t>
+  </si>
+  <si>
+    <t>unordered_set in CPP</t>
+  </si>
+  <si>
+    <t>Use HashSet or Not</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,6 +2579,23 @@
       <c r="D99" t="s">
         <v>270</v>
       </c>
+      <c r="E99" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2154</v>
+      </c>
+      <c r="B100" t="s">
+        <v>271</v>
+      </c>
+      <c r="C100" t="s">
+        <v>230</v>
+      </c>
+      <c r="D100" t="s">
+        <v>273</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">

</xml_diff>

<commit_message>
Set Intersection Size At Least Two.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B89E53-2328-497C-93A6-8106ED42BCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0174C0AF-404B-4DE5-B734-4D5D82706052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="276">
   <si>
     <t>Id</t>
   </si>
@@ -850,6 +850,12 @@
   </si>
   <si>
     <t>Use HashSet or Not</t>
+  </si>
+  <si>
+    <t>Set Intersection Size At Least Two</t>
+  </si>
+  <si>
+    <t>Sort the array of intervals by ascending end, descending start. For each interval, check if has both values, 1 value(let it be the end point), no value(let them be endpoint and endpoint-1)</t>
   </si>
 </sst>
 </file>
@@ -1173,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,6 +2603,20 @@
         <v>273</v>
       </c>
     </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>757</v>
+      </c>
+      <c r="B101" t="s">
+        <v>274</v>
+      </c>
+      <c r="C101" t="s">
+        <v>208</v>
+      </c>
+      <c r="D101" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Unique Length-3 Palindromic Subsequences.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7298E464-038B-4F90-8558-C4681CE52E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D2EDFD-C177-400C-92CF-97145DD1C87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="281">
   <si>
     <t>Id</t>
   </si>
@@ -862,6 +862,15 @@
   </si>
   <si>
     <t>First, second, third; Or sort the array descending O(nlogn)</t>
+  </si>
+  <si>
+    <t>Unique Length-3 Palindromic Subsequences</t>
+  </si>
+  <si>
+    <t>Loop/HashSet</t>
+  </si>
+  <si>
+    <t>Store left most and right most of each character. Loop to check each unique palindromes</t>
   </si>
 </sst>
 </file>
@@ -1185,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,6 +2646,20 @@
         <v>277</v>
       </c>
     </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1930</v>
+      </c>
+      <c r="B103" t="s">
+        <v>278</v>
+      </c>
+      <c r="C103" t="s">
+        <v>279</v>
+      </c>
+      <c r="D103" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Find Minimum Operations To Make All Elements Divisible By Three.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E22D2-F899-4DCE-98B9-0CFC05D5BCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767C6B65-53A4-4C8A-B82B-8211FD826B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="285">
   <si>
     <t>Id</t>
   </si>
@@ -877,6 +877,12 @@
   </si>
   <si>
     <t>Each char digit and carry over, while (m &gt;= 0 || n &gt;=  0 || carry &gt;  0)</t>
+  </si>
+  <si>
+    <t>Find Minimum Operations To Make All Elements Divisible By Three</t>
+  </si>
+  <si>
+    <t>Increase by 1 or Decrease by 1 for each element</t>
   </si>
 </sst>
 </file>
@@ -1200,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,6 +2686,20 @@
         <v>282</v>
       </c>
     </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>3190</v>
+      </c>
+      <c r="B105" t="s">
+        <v>283</v>
+      </c>
+      <c r="C105" t="s">
+        <v>221</v>
+      </c>
+      <c r="D105" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Number Of Segments In A String.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767C6B65-53A4-4C8A-B82B-8211FD826B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C9F06-2812-43AF-AA07-2F805F472B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="287">
   <si>
     <t>Id</t>
   </si>
@@ -883,6 +883,12 @@
   </si>
   <si>
     <t>Increase by 1 or Decrease by 1 for each element</t>
+  </si>
+  <si>
+    <t>Number of Segments in a String</t>
+  </si>
+  <si>
+    <t>Loop and skip ' ', skip non-space and count</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,6 +2706,20 @@
         <v>284</v>
       </c>
     </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>434</v>
+      </c>
+      <c r="B106" t="s">
+        <v>285</v>
+      </c>
+      <c r="C106" t="s">
+        <v>269</v>
+      </c>
+      <c r="D106" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Find All Numbers Disappeared In An Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F00294C-9353-4818-B569-898563448CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33577C33-3E90-41AE-A5B5-88F8D4BC9CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="291">
   <si>
     <t>Id</t>
   </si>
@@ -895,6 +895,12 @@
   </si>
   <si>
     <t>Quadratic functions, 1 + 2 + … + k = n and floor it</t>
+  </si>
+  <si>
+    <t>Find All Numbers Disappeared in an Array</t>
+  </si>
+  <si>
+    <t>Cyclic sort, Swapping values until duplicates</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="C82" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2740,6 +2746,20 @@
         <v>288</v>
       </c>
     </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>448</v>
+      </c>
+      <c r="B108" t="s">
+        <v>289</v>
+      </c>
+      <c r="C108" t="s">
+        <v>208</v>
+      </c>
+      <c r="D108" t="s">
+        <v>290</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Greatest Sum Divisible By Three.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33577C33-3E90-41AE-A5B5-88F8D4BC9CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF595B51-1F86-4411-A321-165E98BDDB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="292">
   <si>
     <t>Id</t>
   </si>
@@ -901,6 +901,9 @@
   </si>
   <si>
     <t>Cyclic sort, Swapping values until duplicates</t>
+  </si>
+  <si>
+    <t>Greatest Sum Divisible by Three</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C82" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,6 +2763,17 @@
         <v>290</v>
       </c>
     </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1262</v>
+      </c>
+      <c r="B109" t="s">
+        <v>291</v>
+      </c>
+      <c r="C109" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Binary Prefix Divisible By Five.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF595B51-1F86-4411-A321-165E98BDDB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B014623-DA94-47BB-B8B6-F33520C05A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="296">
   <si>
     <t>Id</t>
   </si>
@@ -904,6 +904,18 @@
   </si>
   <si>
     <t>Greatest Sum Divisible by Three</t>
+  </si>
+  <si>
+    <t>Binary Prefix Divisible By 5</t>
+  </si>
+  <si>
+    <t>Math/Bitwise</t>
+  </si>
+  <si>
+    <t>Left shift = x2, modulo 5 to prevent overflown because we only care about the last digit</t>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
   </si>
 </sst>
 </file>
@@ -1227,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,6 +2786,31 @@
         <v>252</v>
       </c>
     </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1018</v>
+      </c>
+      <c r="B110" t="s">
+        <v>292</v>
+      </c>
+      <c r="C110" t="s">
+        <v>293</v>
+      </c>
+      <c r="D110" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>7</v>
+      </c>
+      <c r="B111" t="s">
+        <v>295</v>
+      </c>
+      <c r="C111" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Smallest Integer Divisible By K.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B014623-DA94-47BB-B8B6-F33520C05A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46997B1D-CC43-45B9-ADF0-070B790896AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="298">
   <si>
     <t>Id</t>
   </si>
@@ -916,6 +916,12 @@
   </si>
   <si>
     <t>Reverse Integer</t>
+  </si>
+  <si>
+    <t>Smallest Integer Divisible by K</t>
+  </si>
+  <si>
+    <t>From 1 -&gt; current * 10 + 1 find remainder, if the repeated times exceed K, there is no answer because there are only K possible remainders (0 -&gt; K-1)</t>
   </si>
 </sst>
 </file>
@@ -1239,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,6 +2817,20 @@
         <v>221</v>
       </c>
     </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1015</v>
+      </c>
+      <c r="B112" t="s">
+        <v>296</v>
+      </c>
+      <c r="C112" t="s">
+        <v>221</v>
+      </c>
+      <c r="D112" t="s">
+        <v>297</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Paths in Matrix Whose Sum Is Divisible by K.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46997B1D-CC43-45B9-ADF0-070B790896AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5180CD-70E6-4143-8174-90E7133CB115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="300">
   <si>
     <t>Id</t>
   </si>
@@ -922,6 +922,12 @@
   </si>
   <si>
     <t>From 1 -&gt; current * 10 + 1 find remainder, if the repeated times exceed K, there is no answer because there are only K possible remainders (0 -&gt; K-1)</t>
+  </si>
+  <si>
+    <t>Paths in Matrix Whose Sum Is Divisible by K</t>
+  </si>
+  <si>
+    <t>Have a dp[m,n,k]([][][]) to represent the paths that reach cell (m,n) and the remainder of the path sum, traverse each path with m*n*k</t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,6 +2837,20 @@
         <v>297</v>
       </c>
     </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2435</v>
+      </c>
+      <c r="B113" t="s">
+        <v>298</v>
+      </c>
+      <c r="C113" t="s">
+        <v>252</v>
+      </c>
+      <c r="D113" t="s">
+        <v>299</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximum Subarray Sum With Length Divisible by K.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07568688-47F1-4C76-BAA9-7A3459039D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE2D4A9-F54E-476B-93BF-E8F93917D0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="305">
   <si>
     <t>Id</t>
   </si>
@@ -931,6 +931,18 @@
   </si>
   <si>
     <t>If &gt; 2147483641 or &lt; - 2147483641 return 0; use a temp to convert to positive, spread the digits to a list, if &lt; 9 digits then compute normally, else compare with each digits of max int 32-bit, if current is greater and prev is equal then return 0 else compute normally</t>
+  </si>
+  <si>
+    <t>Simply extract digit and compare the current result with the extracted value of MaxInt / 10 and MinInt / 10 before multiplying to the 10th digit.</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum With Length Divisible By K</t>
+  </si>
+  <si>
+    <t>Prefix Sum Array</t>
+  </si>
+  <si>
+    <t>kSum store the min value of the prefixSum in each remainder group from 0 -&gt; k-1 in each element, as long as the length-i prefixSum and the kSum element having the same remainder, their difference will be the length of subarray divisible by K</t>
   </si>
 </sst>
 </file>
@@ -1254,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="E97" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,6 +2840,9 @@
       <c r="D111" t="s">
         <v>300</v>
       </c>
+      <c r="E111" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
@@ -2843,7 +2858,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2435</v>
       </c>
@@ -2855,6 +2870,23 @@
       </c>
       <c r="D113" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>3381</v>
+      </c>
+      <c r="B114" t="s">
+        <v>302</v>
+      </c>
+      <c r="C114" t="s">
+        <v>221</v>
+      </c>
+      <c r="D114" t="s">
+        <v>303</v>
+      </c>
+      <c r="E114" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maximum Number Of K Divisible Components.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE2D4A9-F54E-476B-93BF-E8F93917D0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6FA5E4-6217-4630-86E9-22C8B0B19342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="307">
   <si>
     <t>Id</t>
   </si>
@@ -943,6 +943,12 @@
   </si>
   <si>
     <t>kSum store the min value of the prefixSum in each remainder group from 0 -&gt; k-1 in each element, as long as the length-i prefixSum and the kSum element having the same remainder, their difference will be the length of subarray divisible by K</t>
+  </si>
+  <si>
+    <t>Maximum Number of K-Divisible Components</t>
+  </si>
+  <si>
+    <t>Recursive/DFS</t>
   </si>
 </sst>
 </file>
@@ -1266,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E97" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,6 +2895,17 @@
         <v>304</v>
       </c>
     </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2872</v>
+      </c>
+      <c r="B115" t="s">
+        <v>305</v>
+      </c>
+      <c r="C115" t="s">
+        <v>306</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Add Two Numbers - Minimum Operations to Make Array Sum Divisible by K.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6FA5E4-6217-4630-86E9-22C8B0B19342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72F88B-CB05-4AF5-8481-DFECB62F15DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="312">
   <si>
     <t>Id</t>
   </si>
@@ -949,6 +949,21 @@
   </si>
   <si>
     <t>Recursive/DFS</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t>return dumm.next or break to cut the trail</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Make Array Sum Divisible by K</t>
+  </si>
+  <si>
+    <t>return the remainder of the sum</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="C97" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,6 +2921,34 @@
         <v>306</v>
       </c>
     </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116" t="s">
+        <v>307</v>
+      </c>
+      <c r="C116" t="s">
+        <v>308</v>
+      </c>
+      <c r="D116" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>3512</v>
+      </c>
+      <c r="B117" t="s">
+        <v>310</v>
+      </c>
+      <c r="C117" t="s">
+        <v>221</v>
+      </c>
+      <c r="D117" t="s">
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Longest Substring Without Repeating Characters.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72F88B-CB05-4AF5-8481-DFECB62F15DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B565AE66-E6A3-4733-9F74-2E82EEC4FC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="315">
   <si>
     <t>Id</t>
   </si>
@@ -964,6 +964,15 @@
   </si>
   <si>
     <t>return the remainder of the sum</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>Loop/HashSet/Dictionary</t>
+  </si>
+  <si>
+    <t>Slinding window, HashSet: shrink the left when seen and remove any seen on the path, Dictionary: compare prevIndex witt current left and update the new seen value</t>
   </si>
 </sst>
 </file>
@@ -1287,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C97" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,6 +2958,20 @@
         <v>311</v>
       </c>
     </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118" t="s">
+        <v>312</v>
+      </c>
+      <c r="C118" t="s">
+        <v>313</v>
+      </c>
+      <c r="D118" t="s">
+        <v>314</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Number Of Trapezoids 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B565AE66-E6A3-4733-9F74-2E82EEC4FC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40061E-404D-4CE2-91CC-5A82C5CD9FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="318">
   <si>
     <t>Id</t>
   </si>
@@ -973,6 +973,15 @@
   </si>
   <si>
     <t>Slinding window, HashSet: shrink the left when seen and remove any seen on the path, Dictionary: compare prevIndex witt current left and update the new seen value</t>
+  </si>
+  <si>
+    <t>Count Number of Trapezoids 1</t>
+  </si>
+  <si>
+    <t>Loop/Math/Dictionary</t>
+  </si>
+  <si>
+    <t>Group the points by Y-coordinates in a map/dictionary/unordered_set, iterate by each level with a prefixSum of all previous segments and add to the result</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,6 +2981,20 @@
         <v>314</v>
       </c>
     </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>3623</v>
+      </c>
+      <c r="B119" t="s">
+        <v>315</v>
+      </c>
+      <c r="C119" t="s">
+        <v>316</v>
+      </c>
+      <c r="D119" t="s">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Collisions on a Road.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40061E-404D-4CE2-91CC-5A82C5CD9FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C2D258-5634-4051-87D3-E32BAB76C0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="320">
   <si>
     <t>Id</t>
   </si>
@@ -981,7 +981,13 @@
     <t>Loop/Math/Dictionary</t>
   </si>
   <si>
-    <t>Group the points by Y-coordinates in a map/dictionary/unordered_set, iterate by each level with a prefixSum of all previous segments and add to the result</t>
+    <t>Group the points by Y-coordinates in a map/dictionary/unordered_map, iterate by each level with a prefixSum of all previous segments and add to the result</t>
+  </si>
+  <si>
+    <t>Count Collisions on a Road</t>
+  </si>
+  <si>
+    <t>Trim leading L, Trim trailing R, each non S will be in a collision eventually</t>
   </si>
 </sst>
 </file>
@@ -1305,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2995,6 +3001,20 @@
         <v>317</v>
       </c>
     </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2211</v>
+      </c>
+      <c r="B120" t="s">
+        <v>318</v>
+      </c>
+      <c r="C120" t="s">
+        <v>221</v>
+      </c>
+      <c r="D120" t="s">
+        <v>319</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Partitions with Even Sum Difference.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C2D258-5634-4051-87D3-E32BAB76C0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90814689-F975-4327-A586-06766377F95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="323">
   <si>
     <t>Id</t>
   </si>
@@ -988,6 +988,15 @@
   </si>
   <si>
     <t>Trim leading L, Trim trailing R, each non S will be in a collision eventually</t>
+  </si>
+  <si>
+    <t>Count Partitions with Even Sum Difference</t>
+  </si>
+  <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <t>If total is even, every partition is valid, else 0</t>
   </si>
 </sst>
 </file>
@@ -1311,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="E109" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,6 +3024,23 @@
         <v>319</v>
       </c>
     </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>3432</v>
+      </c>
+      <c r="B121" t="s">
+        <v>320</v>
+      </c>
+      <c r="C121" t="s">
+        <v>221</v>
+      </c>
+      <c r="D121" t="s">
+        <v>321</v>
+      </c>
+      <c r="E121" t="s">
+        <v>322</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Square Sum Triples.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACE2230-F1D6-43CF-8915-83E729DFBDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B78E3F2-F8C6-4DD2-A9EB-35CC64834C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="333">
   <si>
     <t>Id</t>
   </si>
@@ -1015,6 +1015,18 @@
   </si>
   <si>
     <t>Left and Right, advance the lower</t>
+  </si>
+  <si>
+    <t>Count Sum Triples</t>
+  </si>
+  <si>
+    <t>Loop for valid pairs, check if integer and less &lt;= n</t>
+  </si>
+  <si>
+    <t>Iterate thru all possible hypotenous c, 2 pointers approach</t>
+  </si>
+  <si>
+    <t>Math/Loop/2 Pointers</t>
   </si>
 </sst>
 </file>
@@ -1338,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C109" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3090,6 +3102,23 @@
         <v>328</v>
       </c>
     </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1925</v>
+      </c>
+      <c r="B124" t="s">
+        <v>329</v>
+      </c>
+      <c r="C124" t="s">
+        <v>332</v>
+      </c>
+      <c r="D124" t="s">
+        <v>330</v>
+      </c>
+      <c r="E124" t="s">
+        <v>331</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Odd Numbers in an Interval Range.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B78E3F2-F8C6-4DD2-A9EB-35CC64834C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E110A929-F812-4313-ACEC-60E9A03A627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="335">
   <si>
     <t>Id</t>
   </si>
@@ -1027,6 +1027,12 @@
   </si>
   <si>
     <t>Math/Loop/2 Pointers</t>
+  </si>
+  <si>
+    <t>Count Odd Numbers in an Interval Range</t>
+  </si>
+  <si>
+    <t>Difference /2 + 1</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,6 +3125,20 @@
         <v>331</v>
       </c>
     </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1523</v>
+      </c>
+      <c r="B125" t="s">
+        <v>333</v>
+      </c>
+      <c r="C125" t="s">
+        <v>293</v>
+      </c>
+      <c r="D125" t="s">
+        <v>334</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count The Number of Computer Unlocking Permutations.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E110A929-F812-4313-ACEC-60E9A03A627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3771D5DA-165F-455E-A334-5DE300BE36E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="337">
   <si>
     <t>Id</t>
   </si>
@@ -1033,6 +1033,12 @@
   </si>
   <si>
     <t>Difference /2 + 1</t>
+  </si>
+  <si>
+    <t>Count the Number of Computer Unlocking Permutations</t>
+  </si>
+  <si>
+    <t>first index must have smallest value, the rest is permutation.</t>
   </si>
 </sst>
 </file>
@@ -1356,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,6 +3145,20 @@
         <v>334</v>
       </c>
     </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>3577</v>
+      </c>
+      <c r="B126" t="s">
+        <v>335</v>
+      </c>
+      <c r="C126" t="s">
+        <v>221</v>
+      </c>
+      <c r="D126" t="s">
+        <v>336</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Best Time To Buy And Sell Stock V.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179FE840-F3E5-4FDE-AEA9-2AF51CEDE99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A949A4-2715-4B02-8AFA-C4C70FC47E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9105" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="348">
   <si>
     <t>Id</t>
   </si>
@@ -1063,6 +1063,15 @@
   </si>
   <si>
     <t>C++: use lambda and auto auto isValidCode = [](const string&amp; s) {}, isalnum</t>
+  </si>
+  <si>
+    <t>Number of Smooth Descent Period of a Stock</t>
+  </si>
+  <si>
+    <t>Loop/Math/2 Ponters</t>
+  </si>
+  <si>
+    <t>Find each longest periods, count the elements, the total = 1+2+…+k, keep sliding with 2 pointers</t>
   </si>
 </sst>
 </file>
@@ -1104,8 +1113,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E109" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+    <sheetView tabSelected="1" topLeftCell="C109" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,6 +3234,20 @@
         <v>344</v>
       </c>
     </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2110</v>
+      </c>
+      <c r="B130" t="s">
+        <v>345</v>
+      </c>
+      <c r="C130" t="s">
+        <v>346</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Delete Columns To Make Sorted 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A949A4-2715-4B02-8AFA-C4C70FC47E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56111436-2813-4E3E-B4CE-CFE2C1C54026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9105" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="349">
   <si>
     <t>Id</t>
   </si>
@@ -1072,6 +1072,9 @@
   </si>
   <si>
     <t>Find each longest periods, count the elements, the total = 1+2+…+k, keep sliding with 2 pointers</t>
+  </si>
+  <si>
+    <t>Delete Columns To Make Sorted</t>
   </si>
 </sst>
 </file>
@@ -1398,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C109" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3248,6 +3251,17 @@
         <v>347</v>
       </c>
     </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>955</v>
+      </c>
+      <c r="B131" t="s">
+        <v>348</v>
+      </c>
+      <c r="C131" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Delete Columns To Make Sorted 3.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56111436-2813-4E3E-B4CE-CFE2C1C54026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC00F717-1BB4-4119-AD7C-3B9F75F4E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="353">
   <si>
     <t>Id</t>
   </si>
@@ -1074,7 +1074,19 @@
     <t>Find each longest periods, count the elements, the total = 1+2+…+k, keep sliding with 2 pointers</t>
   </si>
   <si>
-    <t>Delete Columns To Make Sorted</t>
+    <t>Delete Columns To Make Sorted 3</t>
+  </si>
+  <si>
+    <t>Delete Columns To Make Sorted 2</t>
+  </si>
+  <si>
+    <t>Loop/Dynamic Progamming</t>
+  </si>
+  <si>
+    <t>Have a dp[cols] to represent the longest length among all row(string) in strs upto index j</t>
+  </si>
+  <si>
+    <t>How many valid characters &lt; character at index j.</t>
   </si>
 </sst>
 </file>
@@ -1401,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="E118" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3256,10 +3268,27 @@
         <v>955</v>
       </c>
       <c r="B131" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C131" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>960</v>
+      </c>
+      <c r="B132" t="s">
+        <v>348</v>
+      </c>
+      <c r="C132" t="s">
+        <v>350</v>
+      </c>
+      <c r="D132" t="s">
+        <v>351</v>
+      </c>
+      <c r="E132" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two Best Non Overlapping Events.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC00F717-1BB4-4119-AD7C-3B9F75F4E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D72200-E7AB-4977-A03A-9C8A5A5ECA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="356">
   <si>
     <t>Id</t>
   </si>
@@ -1086,7 +1086,16 @@
     <t>Have a dp[cols] to represent the longest length among all row(string) in strs upto index j</t>
   </si>
   <si>
-    <t>How many valid characters &lt; character at index j.</t>
+    <t>How many valid characters in the sequence &lt; character at index j.</t>
+  </si>
+  <si>
+    <t>Two Best Non-Overlapping Events</t>
+  </si>
+  <si>
+    <t>Loop/Priority Queue</t>
+  </si>
+  <si>
+    <t>Have a PQ to store all the (value,endTime), Dequeue all the old events that are finished at the current event (current start Time), keep track of the max value already in pq.</t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E118" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,6 +3300,20 @@
         <v>352</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>2054</v>
+      </c>
+      <c r="B133" t="s">
+        <v>353</v>
+      </c>
+      <c r="C133" t="s">
+        <v>354</v>
+      </c>
+      <c r="D133" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximize Happiness Of Selected Children.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D72200-E7AB-4977-A03A-9C8A5A5ECA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE5D7F-E7C3-4DF1-B1B4-3CD96AB0B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="361">
   <si>
     <t>Id</t>
   </si>
@@ -1096,6 +1096,21 @@
   </si>
   <si>
     <t>Have a PQ to store all the (value,endTime), Dequeue all the old events that are finished at the current event (current start Time), keep track of the max value already in pq.</t>
+  </si>
+  <si>
+    <t>Apple Redistribution into Boxes</t>
+  </si>
+  <si>
+    <t>Loop/Greedy</t>
+  </si>
+  <si>
+    <t>Maximize Happiness of Selected Children</t>
+  </si>
+  <si>
+    <t>Sort the capacity descending, greedily put each pack into the bag, conditionally check with the extra space.</t>
+  </si>
+  <si>
+    <t>Sort the happiness descending, greedily take each value and subtract 1 correspondingly, if the value is negative make it 0</t>
   </si>
 </sst>
 </file>
@@ -1422,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,6 +3329,34 @@
         <v>355</v>
       </c>
     </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>3074</v>
+      </c>
+      <c r="B134" t="s">
+        <v>356</v>
+      </c>
+      <c r="C134" t="s">
+        <v>357</v>
+      </c>
+      <c r="D134" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>3075</v>
+      </c>
+      <c r="B135" t="s">
+        <v>358</v>
+      </c>
+      <c r="C135" t="s">
+        <v>357</v>
+      </c>
+      <c r="D135" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Penalty For A Shop.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE5D7F-E7C3-4DF1-B1B4-3CD96AB0B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1DCE55-AD3B-44D5-ADA1-6D6D357846C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="363">
   <si>
     <t>Id</t>
   </si>
@@ -1111,6 +1111,12 @@
   </si>
   <si>
     <t>Sort the happiness descending, greedily take each value and subtract 1 correspondingly, if the value is negative make it 0</t>
+  </si>
+  <si>
+    <t>Minimum Penalty for a Shop</t>
+  </si>
+  <si>
+    <t>Track the penalty or the score with 'Y'</t>
   </si>
 </sst>
 </file>
@@ -1437,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G135"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3357,6 +3363,20 @@
         <v>360</v>
       </c>
     </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2483</v>
+      </c>
+      <c r="B136" t="s">
+        <v>361</v>
+      </c>
+      <c r="C136" t="s">
+        <v>208</v>
+      </c>
+      <c r="D136" t="s">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Count Negative Numbers in a Sorted Matrix.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8838F2-7E50-4AF4-9FCE-E154FBD8C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BECEC3-2A52-4656-A7A1-89C38D4D72D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="367">
   <si>
     <t>Id</t>
   </si>
@@ -1120,6 +1120,15 @@
   </si>
   <si>
     <t>Meeting Room 3</t>
+  </si>
+  <si>
+    <t>Count Negative Numbers in a Sorted Matrix</t>
+  </si>
+  <si>
+    <t>Loop/Binary Search</t>
+  </si>
+  <si>
+    <t>Start from bottom left or top right and add up</t>
   </si>
 </sst>
 </file>
@@ -1446,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3391,6 +3400,20 @@
         <v>354</v>
       </c>
     </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1351</v>
+      </c>
+      <c r="B138" t="s">
+        <v>364</v>
+      </c>
+      <c r="C138" t="s">
+        <v>365</v>
+      </c>
+      <c r="D138" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
N Repeated Element Size Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BECEC3-2A52-4656-A7A1-89C38D4D72D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EC9950-7D25-481A-BA10-F652264AE5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="370">
   <si>
     <t>Id</t>
   </si>
@@ -1129,6 +1129,15 @@
   </si>
   <si>
     <t>Start from bottom left or top right and add up</t>
+  </si>
+  <si>
+    <t>N-Repeated Element in Size 2N Array</t>
+  </si>
+  <si>
+    <t>Loop/Dictionary</t>
+  </si>
+  <si>
+    <t>If the key is already in the dict, return the number</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G138"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3414,6 +3423,20 @@
         <v>366</v>
       </c>
     </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>961</v>
+      </c>
+      <c r="B139" t="s">
+        <v>367</v>
+      </c>
+      <c r="C139" t="s">
+        <v>368</v>
+      </c>
+      <c r="D139" t="s">
+        <v>369</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Number Of Ways to Paint Nx3 Grid.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EC9950-7D25-481A-BA10-F652264AE5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58422BAB-8450-4F9D-B3DA-EA0ED24642EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="372">
   <si>
     <t>Id</t>
   </si>
@@ -1138,6 +1138,12 @@
   </si>
   <si>
     <t>If the key is already in the dict, return the number</t>
+  </si>
+  <si>
+    <t>Number of Ways To Paint Nx3 Grid</t>
+  </si>
+  <si>
+    <t>2 Color Pattern = 6; 3 Color Pattern = 6; figure the pattern in the next row, how many ways are there?</t>
   </si>
 </sst>
 </file>
@@ -1464,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3437,6 +3443,20 @@
         <v>369</v>
       </c>
     </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>1411</v>
+      </c>
+      <c r="B140" t="s">
+        <v>370</v>
+      </c>
+      <c r="C140" t="s">
+        <v>221</v>
+      </c>
+      <c r="D140" t="s">
+        <v>371</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximum Level Sum of a Binary Tree.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77198CA-DF16-4539-9E8D-D1469EC137D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4458BA76-10B9-4A68-9B5F-09201D2119D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="379">
   <si>
     <t>Id</t>
   </si>
@@ -1156,6 +1156,15 @@
   </si>
   <si>
     <t>Count the negative, track min, iterate each cell.</t>
+  </si>
+  <si>
+    <t>Maximum Level Sum of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Loop/TreeNode/Queue</t>
+  </si>
+  <si>
+    <t>Using Queue for BFS and a tuple or KVP to keep track of the current level. Iterate the queue until it has nothing and check for the sum and max and level.</t>
   </si>
 </sst>
 </file>
@@ -1482,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,6 +3506,20 @@
         <v>375</v>
       </c>
     </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1161</v>
+      </c>
+      <c r="B143" t="s">
+        <v>376</v>
+      </c>
+      <c r="C143" t="s">
+        <v>377</v>
+      </c>
+      <c r="D143" t="s">
+        <v>378</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximum Product of Splitted Binary Tree.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4458BA76-10B9-4A68-9B5F-09201D2119D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B6EE56-456D-436A-8E33-1D66E7007EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="382">
   <si>
     <t>Id</t>
   </si>
@@ -1165,6 +1165,15 @@
   </si>
   <si>
     <t>Using Queue for BFS and a tuple or KVP to keep track of the current level. Iterate the queue until it has nothing and check for the sum and max and level.</t>
+  </si>
+  <si>
+    <t>Maximum Product of Splitted Binary Tree</t>
+  </si>
+  <si>
+    <t>Loop/Recursive/TreeNode/Stack/Math</t>
+  </si>
+  <si>
+    <t>DFS(preorder) to find total sum, then DFS(postorder) to compute the sum of each subtree, find the current max.</t>
   </si>
 </sst>
 </file>
@@ -1491,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G143"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3520,6 +3529,20 @@
         <v>378</v>
       </c>
     </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1339</v>
+      </c>
+      <c r="B144" t="s">
+        <v>379</v>
+      </c>
+      <c r="C144" t="s">
+        <v>380</v>
+      </c>
+      <c r="D144" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Smallest Subtree With All The Deepest Nodes.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B6EE56-456D-436A-8E33-1D66E7007EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B1F909-7F73-4FC0-9F33-56266DF3451F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="386">
   <si>
     <t>Id</t>
   </si>
@@ -1174,6 +1174,18 @@
   </si>
   <si>
     <t>DFS(preorder) to find total sum, then DFS(postorder) to compute the sum of each subtree, find the current max.</t>
+  </si>
+  <si>
+    <t>Max Dot Product of Two Subsequences</t>
+  </si>
+  <si>
+    <t>Smallest Subtree with all the Deepest Nodes</t>
+  </si>
+  <si>
+    <t>Loop/Recursive/TreeNode</t>
+  </si>
+  <si>
+    <t>(DEEPEST PARENT NODE of a SUBTREE CONTAINING ALL THE DEEPEST NODES) Find the maxDepth. Traverse the tree,  when it reaches the max depth return the node, if both descendants are not null return the node, or return the descendant that is not null.</t>
   </si>
 </sst>
 </file>
@@ -1500,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3543,6 +3555,31 @@
         <v>381</v>
       </c>
     </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1458</v>
+      </c>
+      <c r="B145" t="s">
+        <v>382</v>
+      </c>
+      <c r="C145" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>865</v>
+      </c>
+      <c r="B146" t="s">
+        <v>383</v>
+      </c>
+      <c r="C146" t="s">
+        <v>384</v>
+      </c>
+      <c r="D146" t="s">
+        <v>385</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Time Visiting All Points.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F16975-ED64-4DED-A7C8-41B1683E0C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954E19A9-7D37-4BD3-9083-587321302B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="390">
   <si>
     <t>Id</t>
   </si>
@@ -1192,6 +1192,12 @@
   </si>
   <si>
     <t>Maximal Rectangle</t>
+  </si>
+  <si>
+    <t>Minimum Time Visiting All Points</t>
+  </si>
+  <si>
+    <t>Add the higher distance.</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,6 +3611,20 @@
         <v>387</v>
       </c>
     </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1266</v>
+      </c>
+      <c r="B149" t="s">
+        <v>388</v>
+      </c>
+      <c r="C149" t="s">
+        <v>221</v>
+      </c>
+      <c r="D149" t="s">
+        <v>389</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximize Area of Square Hole in Grid.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE12C88-DB19-43C4-A37F-1774BD04AAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3BCB08-DE1E-406E-97DC-E45F54EAECAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="394">
   <si>
     <t>Id</t>
   </si>
@@ -1204,6 +1204,12 @@
   </si>
   <si>
     <t>Find low and high, total Area, half it, make a helper function to calculate below area, binaray search with precision.</t>
+  </si>
+  <si>
+    <t>Maximize Area of Square Hole in Grid</t>
+  </si>
+  <si>
+    <t>Sort both array</t>
   </si>
 </sst>
 </file>
@@ -1530,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,6 +3651,20 @@
         <v>391</v>
       </c>
     </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>2943</v>
+      </c>
+      <c r="B151" t="s">
+        <v>392</v>
+      </c>
+      <c r="C151" t="s">
+        <v>221</v>
+      </c>
+      <c r="D151" t="s">
+        <v>393</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximize Square Area by Removing Fences From a Field.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3BCB08-DE1E-406E-97DC-E45F54EAECAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A273AB-ED3F-4645-9E14-735D44623FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2820" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="3360" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="396">
   <si>
     <t>Id</t>
   </si>
@@ -1210,6 +1210,12 @@
   </si>
   <si>
     <t>Sort both array</t>
+  </si>
+  <si>
+    <t>Maximum Square Area by Removing Fences From a Field</t>
+  </si>
+  <si>
+    <t>Add 1st and n-th fences into both array, find the largest common max distance in both to determine the side length of the square.</t>
   </si>
 </sst>
 </file>
@@ -1536,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3665,6 +3671,20 @@
         <v>393</v>
       </c>
     </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2975</v>
+      </c>
+      <c r="B152" t="s">
+        <v>394</v>
+      </c>
+      <c r="C152" t="s">
+        <v>221</v>
+      </c>
+      <c r="D152" t="s">
+        <v>395</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Find the Largest Area of Square Inside Two Rectangles.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A273AB-ED3F-4645-9E14-735D44623FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073627A6-DA6F-49D3-A513-F7B43E73C56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="3360" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="398">
   <si>
     <t>Id</t>
   </si>
@@ -1216,6 +1216,12 @@
   </si>
   <si>
     <t>Add 1st and n-th fences into both array, find the largest common max distance in both to determine the side length of the square.</t>
+  </si>
+  <si>
+    <t>Find the Largest Area of Square Inside Two Rectangles</t>
+  </si>
+  <si>
+    <t>Iterate thru each pair of rec, use bottom-left of 1 and top-right of another to determine overlap(Max of both lefts, bottoms and Min of both tops, rights) , find max square area in that overlapping area.</t>
   </si>
 </sst>
 </file>
@@ -1542,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G152"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3685,6 +3691,20 @@
         <v>395</v>
       </c>
     </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>3047</v>
+      </c>
+      <c r="B153" t="s">
+        <v>396</v>
+      </c>
+      <c r="C153" t="s">
+        <v>221</v>
+      </c>
+      <c r="D153" t="s">
+        <v>397</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Maximum Side Length of a Square with Sum Less than or Equal to Threshold.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D609F708-18C5-4ACA-A695-C787AAF77D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B755C4C1-69A9-4DE8-BD7D-092F74EBF6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="2970" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="402">
   <si>
     <t>Id</t>
   </si>
@@ -1228,6 +1228,12 @@
   </si>
   <si>
     <t>Test every square matrix in the grid with PrefixSum for rows and columns</t>
+  </si>
+  <si>
+    <t>Maximum Side Length of a Square with Sum Less than or Equal to Threshold</t>
+  </si>
+  <si>
+    <t>PrefixRow and PrefixCol, at every element grow with extra bottom and right layer and remove bottom right corner duplicate, check the sum.</t>
   </si>
 </sst>
 </file>
@@ -1554,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G154"/>
+  <dimension ref="A1:G155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3725,6 +3731,20 @@
         <v>399</v>
       </c>
     </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1292</v>
+      </c>
+      <c r="B155" t="s">
+        <v>400</v>
+      </c>
+      <c r="C155" t="s">
+        <v>221</v>
+      </c>
+      <c r="D155" t="s">
+        <v>401</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Construct the Minimum Bitwise Array 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B755C4C1-69A9-4DE8-BD7D-092F74EBF6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E082AFFA-7F31-4D6E-88E0-EE485F9E8E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2970" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="403">
   <si>
     <t>Id</t>
   </si>
@@ -1234,6 +1234,9 @@
   </si>
   <si>
     <t>PrefixRow and PrefixCol, at every element grow with extra bottom and right layer and remove bottom right corner duplicate, check the sum.</t>
+  </si>
+  <si>
+    <t>Construct the Minimum Bitwise Array 1</t>
   </si>
 </sst>
 </file>
@@ -1560,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3745,6 +3748,17 @@
         <v>401</v>
       </c>
     </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>3314</v>
+      </c>
+      <c r="B156" t="s">
+        <v>402</v>
+      </c>
+      <c r="C156" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Construct the Minimum Bitwise Array 2.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E082AFFA-7F31-4D6E-88E0-EE485F9E8E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFF6071-DBE5-4596-BF9E-280BEAB2F8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2970" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="406">
   <si>
     <t>Id</t>
   </si>
@@ -1237,6 +1237,15 @@
   </si>
   <si>
     <t>Construct the Minimum Bitwise Array 1</t>
+  </si>
+  <si>
+    <t>Loop/Math/Bitwise</t>
+  </si>
+  <si>
+    <t>Bruteforce to find the j in the range of the constraints or use bitwise: loop until the lowest 0, leftshift</t>
+  </si>
+  <si>
+    <t>use bitwise: loop until the lowest 0, leftshift</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G156"/>
+  <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,7 +3765,24 @@
         <v>402</v>
       </c>
       <c r="C156" t="s">
-        <v>221</v>
+        <v>403</v>
+      </c>
+      <c r="D156" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>3315</v>
+      </c>
+      <c r="B157" t="s">
+        <v>402</v>
+      </c>
+      <c r="C157" t="s">
+        <v>403</v>
+      </c>
+      <c r="D157" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minimum Pair Removal to Sort Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFF6071-DBE5-4596-BF9E-280BEAB2F8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBBF39F-3F05-4FA6-A9D2-75225DB0FEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="2970" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="3525" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="408">
   <si>
     <t>Id</t>
   </si>
@@ -1246,6 +1246,12 @@
   </si>
   <si>
     <t>use bitwise: loop until the lowest 0, leftshift</t>
+  </si>
+  <si>
+    <t>Minimum Pair Removal to Sort Array 1</t>
+  </si>
+  <si>
+    <t>Simulate the process, scan all to check sorted state, scan all the find min sum and replace</t>
   </si>
 </sst>
 </file>
@@ -1572,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+      <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,6 +3791,20 @@
         <v>405</v>
       </c>
     </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>3507</v>
+      </c>
+      <c r="B158" t="s">
+        <v>406</v>
+      </c>
+      <c r="C158" t="s">
+        <v>221</v>
+      </c>
+      <c r="D158" t="s">
+        <v>407</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimizie Maximum Pair Sum in Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBBF39F-3F05-4FA6-A9D2-75225DB0FEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A195DC-D3F0-41A2-A2F7-C08C4EEB15D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="3525" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="410">
   <si>
     <t>Id</t>
   </si>
@@ -1252,6 +1252,12 @@
   </si>
   <si>
     <t>Simulate the process, scan all to check sorted state, scan all the find min sum and replace</t>
+  </si>
+  <si>
+    <t>Minimize Maximum Pair Sum in Array</t>
+  </si>
+  <si>
+    <t>Sort and shrink left right for max sum.</t>
   </si>
 </sst>
 </file>
@@ -1578,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3805,6 +3811,20 @@
         <v>407</v>
       </c>
     </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>1877</v>
+      </c>
+      <c r="B159" t="s">
+        <v>408</v>
+      </c>
+      <c r="C159" t="s">
+        <v>221</v>
+      </c>
+      <c r="D159" t="s">
+        <v>409</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Difference Between Highest and Lowest of K Scores.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A195DC-D3F0-41A2-A2F7-C08C4EEB15D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F8D656-A98C-482F-943E-F45B270C9CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3210" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="412">
   <si>
     <t>Id</t>
   </si>
@@ -1258,6 +1258,12 @@
   </si>
   <si>
     <t>Sort and shrink left right for max sum.</t>
+  </si>
+  <si>
+    <t>Minimum Difference Between Highest and Lowest of K Scores</t>
+  </si>
+  <si>
+    <t>Sort Array and find the min diff</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3825,6 +3831,20 @@
         <v>409</v>
       </c>
     </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1984</v>
+      </c>
+      <c r="B160" t="s">
+        <v>410</v>
+      </c>
+      <c r="C160" t="s">
+        <v>221</v>
+      </c>
+      <c r="D160" t="s">
+        <v>411</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Cost Path with Edge Reversals.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8049F8-AE5D-4607-9FF1-F54E83F2EDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1281ED-AEB1-41A5-A8DD-A633D7BEE64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="3030" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="1230" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="417">
   <si>
     <t>Id</t>
   </si>
@@ -1267,6 +1267,18 @@
   </si>
   <si>
     <t>Minimum Absolute Difference</t>
+  </si>
+  <si>
+    <t>Sort, find min, sweep and add pair</t>
+  </si>
+  <si>
+    <t>Minimum Cost Path with Edge Reversals</t>
+  </si>
+  <si>
+    <t>Loop/Deque/Math/BFS</t>
+  </si>
+  <si>
+    <t>Build an adjacency list of each node, normal flow at the current nod = current cost, reversed flow at the destination node = double cost, dist[] to track the distance, LinkedList for Deque</t>
   </si>
 </sst>
 </file>
@@ -1593,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="C139" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3848,7 +3860,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1200</v>
       </c>
@@ -3857,6 +3869,23 @@
       </c>
       <c r="C161" t="s">
         <v>316</v>
+      </c>
+      <c r="D161" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>3650</v>
+      </c>
+      <c r="B162" t="s">
+        <v>414</v>
+      </c>
+      <c r="C162" t="s">
+        <v>415</v>
+      </c>
+      <c r="D162" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minimum Cost to Convert String 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1281ED-AEB1-41A5-A8DD-A633D7BEE64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B7CE24-8157-491B-BB79-CAB4149B3BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4380" yWindow="1230" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="420">
   <si>
     <t>Id</t>
   </si>
@@ -1278,7 +1278,16 @@
     <t>Loop/Deque/Math/BFS</t>
   </si>
   <si>
-    <t>Build an adjacency list of each node, normal flow at the current nod = current cost, reversed flow at the destination node = double cost, dist[] to track the distance, LinkedList for Deque</t>
+    <t>Build an adjacency list of each node, normal flow at the current nod = current cost, reversed flow at the destination node = double cost, dist[] to track the distance, LinkedList for Deque, BFS for min Distance</t>
+  </si>
+  <si>
+    <t>Minimum Cost to Convert String 1</t>
+  </si>
+  <si>
+    <t>Loop/Dictionary/Math</t>
+  </si>
+  <si>
+    <t>Graph of (26,26) to map all conversion possibilities, same character = 0, other assign a huge value, populate the cost. Then Floyd-Warshall for every intermediate char, can I convert this char to that char (26^3). Finally, iterate thru the original and the changed to determine the cost</t>
   </si>
 </sst>
 </file>
@@ -1605,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C139" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3888,6 +3897,20 @@
         <v>416</v>
       </c>
     </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>2976</v>
+      </c>
+      <c r="B163" t="s">
+        <v>417</v>
+      </c>
+      <c r="C163" t="s">
+        <v>418</v>
+      </c>
+      <c r="D163" t="s">
+        <v>419</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Find Smallest Letter Greater Than Target.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B7CE24-8157-491B-BB79-CAB4149B3BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768C3493-9628-45CA-B8F7-B5074F1DBAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="1230" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="421">
   <si>
     <t>Id</t>
   </si>
@@ -1288,6 +1288,9 @@
   </si>
   <si>
     <t>Graph of (26,26) to map all conversion possibilities, same character = 0, other assign a huge value, populate the cost. Then Floyd-Warshall for every intermediate char, can I convert this char to that char (26^3). Finally, iterate thru the original and the changed to determine the cost</t>
+  </si>
+  <si>
+    <t>Find Smallest Letter Greater than Target</t>
   </si>
 </sst>
 </file>
@@ -1614,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G163"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C139" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3911,6 +3914,20 @@
         <v>419</v>
       </c>
     </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>744</v>
+      </c>
+      <c r="B164" t="s">
+        <v>420</v>
+      </c>
+      <c r="C164" t="s">
+        <v>365</v>
+      </c>
+      <c r="D164" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Divide An Array Into Subarrays With Minimum Cost 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768C3493-9628-45CA-B8F7-B5074F1DBAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1445F4-A867-431A-A23C-B53C37EAEAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="424">
   <si>
     <t>Id</t>
   </si>
@@ -1291,6 +1291,15 @@
   </si>
   <si>
     <t>Find Smallest Letter Greater than Target</t>
+  </si>
+  <si>
+    <t>Divide an Array Into Subarrays with Minimum Cost 1</t>
+  </si>
+  <si>
+    <t>Loop/Math/2 Pointers</t>
+  </si>
+  <si>
+    <t>First element is fixed, find the 2 mins value. Sorting or loop with 2 pointers</t>
   </si>
 </sst>
 </file>
@@ -1617,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,6 +3937,20 @@
         <v>145</v>
       </c>
     </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>3010</v>
+      </c>
+      <c r="B165" t="s">
+        <v>421</v>
+      </c>
+      <c r="C165" t="s">
+        <v>422</v>
+      </c>
+      <c r="D165" t="s">
+        <v>423</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Removals To Balance Array.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C635EAC8-1DC5-41B0-85B7-2C2C17A92440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C7E083-C91E-4905-89FC-78714A00BE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="2265" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="430">
   <si>
     <t>Id</t>
   </si>
@@ -1312,6 +1312,12 @@
   </si>
   <si>
     <t>Simulate the process for the circular rotaion. OR use modulus</t>
+  </si>
+  <si>
+    <t>Minimum Removals to Balance Array</t>
+  </si>
+  <si>
+    <t>Sort and use sliding windows to expand the window, check for the min</t>
   </si>
 </sst>
 </file>
@@ -1638,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C139" workbookViewId="0">
-      <selection activeCell="D167" sqref="D167"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3991,6 +3997,20 @@
         <v>427</v>
       </c>
     </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>3634</v>
+      </c>
+      <c r="B168" t="s">
+        <v>428</v>
+      </c>
+      <c r="C168" t="s">
+        <v>221</v>
+      </c>
+      <c r="D168" t="s">
+        <v>429</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Minimum Deletions to Make String Balanced.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C7E083-C91E-4905-89FC-78714A00BE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C134CE3-7CCF-44DA-BD04-BCED68B3266A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="433">
   <si>
     <t>Id</t>
   </si>
@@ -1318,6 +1318,15 @@
   </si>
   <si>
     <t>Sort and use sliding windows to expand the window, check for the min</t>
+  </si>
+  <si>
+    <t>Minimum Deletions to Make String Balance</t>
+  </si>
+  <si>
+    <t>First pass to find aCount and bCount. Second pass from the left, if 'a' reduce a count else increase b count check min of current min and sum acount + bcount</t>
+  </si>
+  <si>
+    <t>Also, have bCount and deletionCount. 1 Pass to increase bCount else find min of deletion and bCount</t>
   </si>
 </sst>
 </file>
@@ -1644,10 +1653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+    <sheetView tabSelected="1" topLeftCell="E139" workbookViewId="0">
+      <selection activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3899,7 +3908,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1200</v>
       </c>
@@ -3913,7 +3922,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>3650</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2976</v>
       </c>
@@ -3941,7 +3950,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>744</v>
       </c>
@@ -3955,7 +3964,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>3010</v>
       </c>
@@ -3969,7 +3978,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>3637</v>
       </c>
@@ -3983,7 +3992,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>3379</v>
       </c>
@@ -3997,7 +4006,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>3634</v>
       </c>
@@ -4009,6 +4018,23 @@
       </c>
       <c r="D168" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1653</v>
+      </c>
+      <c r="B169" t="s">
+        <v>430</v>
+      </c>
+      <c r="C169" t="s">
+        <v>221</v>
+      </c>
+      <c r="D169" t="s">
+        <v>431</v>
+      </c>
+      <c r="E169" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balance A Binary Search Tree.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBAEE4D-4C54-4A53-B49C-698B9E698B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4897813A-B2C3-48E8-B5F4-BF4048B74689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7245" yWindow="1575" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="437">
   <si>
     <t>Id</t>
   </si>
@@ -1333,6 +1333,12 @@
   </si>
   <si>
     <t>DFS(postorder) to return the height, return the flag -1 if the subtrees are unbalanced by checking the diff between lHeight and rHeight, else return the height</t>
+  </si>
+  <si>
+    <t>Balance a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>In-order Traversal to collect and sort the nodes, then build a balance tree with left right mid evenly</t>
   </si>
 </sst>
 </file>
@@ -1659,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C160" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,6 +4063,20 @@
         <v>434</v>
       </c>
     </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1382</v>
+      </c>
+      <c r="B171" t="s">
+        <v>435</v>
+      </c>
+      <c r="C171" t="s">
+        <v>306</v>
+      </c>
+      <c r="D171" t="s">
+        <v>436</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Longest Balanced Substring 1.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4897813A-B2C3-48E8-B5F4-BF4048B74689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6C2C81-2525-46ED-983D-52D527A494B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7245" yWindow="1575" windowWidth="19695" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="443">
   <si>
     <t>Id</t>
   </si>
@@ -1339,6 +1339,24 @@
   </si>
   <si>
     <t>In-order Traversal to collect and sort the nodes, then build a balance tree with left right mid evenly</t>
+  </si>
+  <si>
+    <t>Longest Balanced Subarray 1</t>
+  </si>
+  <si>
+    <t>Math/Dictionary/HashSet</t>
+  </si>
+  <si>
+    <t>Sliding window, count.</t>
+  </si>
+  <si>
+    <t>Longest Balanced Substring 1</t>
+  </si>
+  <si>
+    <t>Math/Dictionary</t>
+  </si>
+  <si>
+    <t>Bruteforce all the substring and iterate the dictionary to test isBalanced.</t>
   </si>
 </sst>
 </file>
@@ -1665,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C160" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4077,6 +4095,34 @@
         <v>436</v>
       </c>
     </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>3719</v>
+      </c>
+      <c r="B172" t="s">
+        <v>437</v>
+      </c>
+      <c r="C172" t="s">
+        <v>438</v>
+      </c>
+      <c r="D172" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>3713</v>
+      </c>
+      <c r="B173" t="s">
+        <v>440</v>
+      </c>
+      <c r="C173" t="s">
+        <v>441</v>
+      </c>
+      <c r="D173" t="s">
+        <v>442</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Binary Number With Alternating Bits.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060CFCCB-8B8E-46E2-8389-920E30E97F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD009E-F0A9-47AD-9A23-78004043F6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="451">
   <si>
     <t>Id</t>
   </si>
@@ -1372,6 +1372,15 @@
   </si>
   <si>
     <t>Count prevGroup and currentGroup of consecutive same bit, add the min to the result because the number of groups equals to the elements in the group</t>
+  </si>
+  <si>
+    <t>Binary Number with Alternating Bits</t>
+  </si>
+  <si>
+    <t>Bitwise/Math</t>
+  </si>
+  <si>
+    <t>Extract last bit first, shift and while loop to check.</t>
   </si>
 </sst>
 </file>
@@ -1698,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,6 +4175,20 @@
         <v>447</v>
       </c>
     </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>639</v>
+      </c>
+      <c r="B176" t="s">
+        <v>448</v>
+      </c>
+      <c r="C176" t="s">
+        <v>449</v>
+      </c>
+      <c r="D176" t="s">
+        <v>450</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>

<commit_message>
Prime Number of Set Bits in Binary Representation.
</commit_message>
<xml_diff>
--- a/Pseudo.xlsx
+++ b/Pseudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LC_Solutions\LC_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD009E-F0A9-47AD-9A23-78004043F6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D847C94B-C034-4091-A3EE-9756A502E613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="453">
   <si>
     <t>Id</t>
   </si>
@@ -1381,6 +1381,12 @@
   </si>
   <si>
     <t>Extract last bit first, shift and while loop to check.</t>
+  </si>
+  <si>
+    <t>Prime Number of Set Bits in Binary Representation</t>
+  </si>
+  <si>
+    <t>util countsetbits, util isPrime. There is also a prime mask</t>
   </si>
 </sst>
 </file>
@@ -1707,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,6 +4195,20 @@
         <v>450</v>
       </c>
     </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>762</v>
+      </c>
+      <c r="B177" t="s">
+        <v>451</v>
+      </c>
+      <c r="C177" t="s">
+        <v>449</v>
+      </c>
+      <c r="D177" t="s">
+        <v>452</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
     <sortCondition ref="A2:A54"/>

</xml_diff>